<commit_message>
Moved some files into src, slight modifications and fixes/patches to scraper
</commit_message>
<xml_diff>
--- a/Docs/HistoryScrapeStatus.xlsx
+++ b/Docs/HistoryScrapeStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpete\Documents\Projects\CarStats\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E2245F-3CB4-4E0B-804D-050FCE0DE9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449BB051-16CE-4BDF-9E95-0AEE77ACD209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-3945" windowWidth="29040" windowHeight="15840" xr2:uid="{84160147-604C-44EB-89D6-C5A3DE91A955}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>Index</t>
   </si>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t>History Scrape Status</t>
+  </si>
+  <si>
+    <t>Not counting bad links</t>
   </si>
 </sst>
 </file>
@@ -657,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2B1DA9D-AC09-4F91-8BA6-4CCF32CADB06}">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -670,9 +673,10 @@
     <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -686,7 +690,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -698,34 +702,37 @@
       <c r="I2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="2"/>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="2"/>
       <c r="H4" s="3"/>
       <c r="I4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -734,7 +741,7 @@
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -743,7 +750,7 @@
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -752,7 +759,7 @@
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -761,7 +768,7 @@
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -770,7 +777,7 @@
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -779,7 +786,7 @@
       </c>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -788,7 +795,7 @@
       </c>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -797,7 +804,7 @@
       </c>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -806,7 +813,7 @@
       </c>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -815,7 +822,7 @@
       </c>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -824,7 +831,7 @@
       </c>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1308,7 +1315,7 @@
       <c r="B69" t="s">
         <v>69</v>
       </c>
-      <c r="C69" s="3"/>
+      <c r="C69" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
More bug 'fixes' in scraper
</commit_message>
<xml_diff>
--- a/Docs/HistoryScrapeStatus.xlsx
+++ b/Docs/HistoryScrapeStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpete\Documents\Projects\CarStats\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449BB051-16CE-4BDF-9E95-0AEE77ACD209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E96CEDA-34E4-40ED-9462-3F29BD2BC3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-3945" windowWidth="29040" windowHeight="15840" xr2:uid="{84160147-604C-44EB-89D6-C5A3DE91A955}"/>
   </bookViews>
@@ -662,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2B1DA9D-AC09-4F91-8BA6-4CCF32CADB06}">
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1279,7 +1279,7 @@
       <c r="B65" t="s">
         <v>65</v>
       </c>
-      <c r="C65" s="3"/>
+      <c r="C65" s="2"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">

</xml_diff>

<commit_message>
Maybe like 2/3 done scrapping. Slight modifications to usability of algorithms.
</commit_message>
<xml_diff>
--- a/Docs/HistoryScrapeStatus.xlsx
+++ b/Docs/HistoryScrapeStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpete\Documents\Projects\CarStats\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FFCD6C0-3275-45A9-94AD-3B2D4FF3CDF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4A1E79-8BBC-40FC-9FA1-14D53218C8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-3945" windowWidth="29040" windowHeight="15840" xr2:uid="{84160147-604C-44EB-89D6-C5A3DE91A955}"/>
   </bookViews>
@@ -260,17 +260,17 @@
     <t>Not Done</t>
   </si>
   <si>
-    <t>History Scrape Status</t>
-  </si>
-  <si>
     <t>Not counting bad links</t>
+  </si>
+  <si>
+    <t>History Status (up to 22/23)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,6 +295,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -338,11 +345,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -663,30 +671,30 @@
   <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="C1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>70</v>
       </c>
     </row>
@@ -703,7 +711,7 @@
         <v>71</v>
       </c>
       <c r="J2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -748,7 +756,7 @@
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -784,7 +792,7 @@
       <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -838,7 +846,7 @@
       <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
@@ -901,7 +909,7 @@
       <c r="B23" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="3"/>
+      <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
@@ -910,7 +918,7 @@
       <c r="B24" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="3"/>
+      <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
@@ -919,7 +927,7 @@
       <c r="B25" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="3"/>
+      <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
@@ -928,7 +936,7 @@
       <c r="B26" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="3"/>
+      <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
@@ -946,7 +954,7 @@
       <c r="B28" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="3"/>
+      <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
@@ -955,7 +963,7 @@
       <c r="B29" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="3"/>
+      <c r="C29" s="2"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
@@ -973,7 +981,7 @@
       <c r="B31" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="3"/>
+      <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
@@ -991,7 +999,7 @@
       <c r="B33" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="3"/>
+      <c r="C33" s="2"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
@@ -1009,7 +1017,7 @@
       <c r="B35" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="3"/>
+      <c r="C35" s="2"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
@@ -1018,7 +1026,7 @@
       <c r="B36" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="3"/>
+      <c r="C36" s="2"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
@@ -1027,7 +1035,7 @@
       <c r="B37" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="3"/>
+      <c r="C37" s="2"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
@@ -1045,7 +1053,7 @@
       <c r="B39" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="3"/>
+      <c r="C39" s="2"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
@@ -1054,7 +1062,7 @@
       <c r="B40" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="3"/>
+      <c r="C40" s="1"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
@@ -1117,7 +1125,7 @@
       <c r="B47" t="s">
         <v>47</v>
       </c>
-      <c r="C47" s="3"/>
+      <c r="C47" s="2"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
@@ -1126,7 +1134,7 @@
       <c r="B48" t="s">
         <v>48</v>
       </c>
-      <c r="C48" s="3"/>
+      <c r="C48" s="2"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
@@ -1135,7 +1143,7 @@
       <c r="B49" t="s">
         <v>49</v>
       </c>
-      <c r="C49" s="3"/>
+      <c r="C49" s="2"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
@@ -1144,7 +1152,7 @@
       <c r="B50" t="s">
         <v>50</v>
       </c>
-      <c r="C50" s="3"/>
+      <c r="C50" s="2"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
@@ -1153,7 +1161,7 @@
       <c r="B51" t="s">
         <v>51</v>
       </c>
-      <c r="C51" s="3"/>
+      <c r="C51" s="2"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
@@ -1162,7 +1170,7 @@
       <c r="B52" t="s">
         <v>52</v>
       </c>
-      <c r="C52" s="3"/>
+      <c r="C52" s="2"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
@@ -1180,7 +1188,7 @@
       <c r="B54" t="s">
         <v>54</v>
       </c>
-      <c r="C54" s="3"/>
+      <c r="C54" s="2"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
@@ -1189,7 +1197,7 @@
       <c r="B55" t="s">
         <v>55</v>
       </c>
-      <c r="C55" s="3"/>
+      <c r="C55" s="2"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
@@ -1198,7 +1206,7 @@
       <c r="B56" t="s">
         <v>56</v>
       </c>
-      <c r="C56" s="3"/>
+      <c r="C56" s="2"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
@@ -1207,7 +1215,7 @@
       <c r="B57" t="s">
         <v>57</v>
       </c>
-      <c r="C57" s="3"/>
+      <c r="C57" s="2"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
@@ -1234,7 +1242,7 @@
       <c r="B60" t="s">
         <v>60</v>
       </c>
-      <c r="C60" s="3"/>
+      <c r="C60" s="2"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
@@ -1243,7 +1251,7 @@
       <c r="B61" t="s">
         <v>61</v>
       </c>
-      <c r="C61" s="3"/>
+      <c r="C61" s="2"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
@@ -1252,7 +1260,7 @@
       <c r="B62" t="s">
         <v>62</v>
       </c>
-      <c r="C62" s="3"/>
+      <c r="C62" s="2"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
@@ -1261,7 +1269,7 @@
       <c r="B63" t="s">
         <v>63</v>
       </c>
-      <c r="C63" s="3"/>
+      <c r="C63" s="2"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
@@ -1270,7 +1278,7 @@
       <c r="B64" t="s">
         <v>64</v>
       </c>
-      <c r="C64" s="3"/>
+      <c r="C64" s="2"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
@@ -1297,7 +1305,7 @@
       <c r="B67" t="s">
         <v>67</v>
       </c>
-      <c r="C67" s="3"/>
+      <c r="C67" s="2"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68">
@@ -1306,7 +1314,7 @@
       <c r="B68" t="s">
         <v>68</v>
       </c>
-      <c r="C68" s="3"/>
+      <c r="C68" s="2"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69">
@@ -1319,5 +1327,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Links, almost done scraping. Added python files for scripts in phase 2, updated TODO.txt. Bug fixes in Targets.py and SummaryGenerator.py
</commit_message>
<xml_diff>
--- a/Docs/HistoryScrapeStatus.xlsx
+++ b/Docs/HistoryScrapeStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpete\Documents\Projects\CarStats\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4A1E79-8BBC-40FC-9FA1-14D53218C8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA9AB89-6413-40D4-A96F-BA1690DF8ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-3945" windowWidth="29040" windowHeight="15840" xr2:uid="{84160147-604C-44EB-89D6-C5A3DE91A955}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>Index</t>
   </si>
@@ -251,19 +251,22 @@
     <t>Key</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>In Progress</t>
   </si>
   <si>
     <t>Not Done</t>
   </si>
   <si>
-    <t>Not counting bad links</t>
-  </si>
-  <si>
-    <t>History Status (up to 22/23)</t>
+    <t>History Status</t>
+  </si>
+  <si>
+    <t>Done (not counting bad links)</t>
+  </si>
+  <si>
+    <t>Size (links)</t>
+  </si>
+  <si>
+    <t>Afeela</t>
   </si>
 </sst>
 </file>
@@ -668,20 +671,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2B1DA9D-AC09-4F91-8BA6-4CCF32CADB06}">
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="K51" sqref="K51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -694,7 +698,10 @@
       <c r="C1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="D1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>70</v>
       </c>
     </row>
@@ -705,11 +712,11 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" t="s">
-        <v>71</v>
-      </c>
+      <c r="C2">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="I2" s="2"/>
       <c r="J2" t="s">
         <v>74</v>
       </c>
@@ -719,12 +726,15 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="H3" s="1"/>
-      <c r="I3" t="s">
-        <v>72</v>
+        <v>76</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="I3" s="1"/>
+      <c r="J3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -732,12 +742,15 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="H4" s="3"/>
-      <c r="I4" t="s">
-        <v>73</v>
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="I4" s="3"/>
+      <c r="J4" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -745,585 +758,789 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>39</v>
+      </c>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>43</v>
+      </c>
+      <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>13</v>
+      </c>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>22</v>
+      </c>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>40</v>
+      </c>
+      <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>18</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>37</v>
+      </c>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>11</v>
+      </c>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>19</v>
+      </c>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>33</v>
+      </c>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>17</v>
+      </c>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="3"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>14</v>
+      </c>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="2"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>16</v>
+      </c>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="2"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <v>25</v>
+      </c>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="2"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" s="3"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <v>7</v>
+      </c>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" s="2"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <v>14</v>
+      </c>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="3"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>21</v>
+      </c>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" s="2"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <v>12</v>
+      </c>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" s="2"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
-      </c>
-      <c r="C37" s="2"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <v>6</v>
+      </c>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" s="2"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" s="2"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="C39">
+        <v>9</v>
+      </c>
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
-      </c>
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <v>18</v>
+      </c>
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
-      </c>
-      <c r="C41" s="3"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <v>14</v>
+      </c>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
-      </c>
-      <c r="C42" s="3"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="C42">
+        <v>29</v>
+      </c>
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
-      </c>
-      <c r="C43" s="3"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="C43">
+        <v>46</v>
+      </c>
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
-      </c>
-      <c r="C44" s="3"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="C44">
+        <v>7</v>
+      </c>
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
-      </c>
-      <c r="C45" s="3"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>46</v>
-      </c>
-      <c r="C46" s="3"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="C46">
+        <v>13</v>
+      </c>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>47</v>
-      </c>
-      <c r="C47" s="2"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="C47">
+        <v>12</v>
+      </c>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>48</v>
-      </c>
-      <c r="C48" s="2"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>49</v>
-      </c>
-      <c r="C49" s="2"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="C49">
+        <v>24</v>
+      </c>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>50</v>
-      </c>
-      <c r="C50" s="2"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>51</v>
-      </c>
-      <c r="C51" s="2"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="C51">
+        <v>6</v>
+      </c>
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>52</v>
-      </c>
-      <c r="C52" s="2"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>53</v>
-      </c>
-      <c r="C53" s="3"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="C53">
+        <v>20</v>
+      </c>
+      <c r="D53" s="2"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>54</v>
-      </c>
-      <c r="C54" s="2"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="C54">
+        <v>7</v>
+      </c>
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>55</v>
-      </c>
-      <c r="C55" s="2"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" s="2"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>56</v>
-      </c>
-      <c r="C56" s="2"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>57</v>
-      </c>
-      <c r="C57" s="2"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="C57">
+        <v>7</v>
+      </c>
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>58</v>
-      </c>
-      <c r="C58" s="3"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+      <c r="C58">
+        <v>3</v>
+      </c>
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>59</v>
-      </c>
-      <c r="C59" s="3"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="C59">
+        <v>4</v>
+      </c>
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>60</v>
-      </c>
-      <c r="C60" s="2"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="C60">
+        <v>6</v>
+      </c>
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>61</v>
-      </c>
-      <c r="C61" s="2"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="C61">
+        <v>2</v>
+      </c>
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>62</v>
-      </c>
-      <c r="C62" s="2"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+      <c r="C62">
+        <v>2</v>
+      </c>
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>63</v>
-      </c>
-      <c r="C63" s="2"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63" s="2"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>64</v>
-      </c>
-      <c r="C64" s="2"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="C64">
+        <v>11</v>
+      </c>
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>65</v>
-      </c>
-      <c r="C65" s="2"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="C65">
+        <v>4</v>
+      </c>
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>66</v>
-      </c>
-      <c r="C66" s="2"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="C66">
+        <v>6</v>
+      </c>
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>67</v>
-      </c>
-      <c r="C67" s="2"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="C67">
+        <v>35</v>
+      </c>
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>68</v>
-      </c>
-      <c r="C68" s="2"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="C68">
+        <v>4</v>
+      </c>
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
       <c r="B69" t="s">
+        <v>68</v>
+      </c>
+      <c r="C69">
+        <v>25</v>
+      </c>
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
         <v>69</v>
       </c>
-      <c r="C69" s="2"/>
+      <c r="C70">
+        <v>18</v>
+      </c>
+      <c r="D70" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Done main scraping. Next task: helper scripts and bad link scraping
</commit_message>
<xml_diff>
--- a/Docs/HistoryScrapeStatus.xlsx
+++ b/Docs/HistoryScrapeStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpete\Documents\Projects\CarStats\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA9AB89-6413-40D4-A96F-BA1690DF8ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D838CD7-4541-466E-9BA2-669EE6F9E5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-3945" windowWidth="29040" windowHeight="15840" xr2:uid="{84160147-604C-44EB-89D6-C5A3DE91A955}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>Index</t>
   </si>
@@ -260,13 +260,19 @@
     <t>History Status</t>
   </si>
   <si>
-    <t>Done (not counting bad links)</t>
-  </si>
-  <si>
     <t>Size (links)</t>
   </si>
   <si>
     <t>Afeela</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Error Link Handling</t>
+  </si>
+  <si>
+    <t>Buggy links all over the place</t>
   </si>
 </sst>
 </file>
@@ -673,16 +679,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2B1DA9D-AC09-4F91-8BA6-4CCF32CADB06}">
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="K51" sqref="K51"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="K58" sqref="K58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.44140625" bestFit="1" customWidth="1"/>
@@ -696,10 +703,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>73</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>70</v>
@@ -716,9 +726,10 @@
         <v>11</v>
       </c>
       <c r="D2" s="2"/>
+      <c r="E2" s="3"/>
       <c r="I2" s="2"/>
       <c r="J2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -726,12 +737,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" s="2"/>
+      <c r="E3" s="3"/>
       <c r="I3" s="1"/>
       <c r="J3" t="s">
         <v>71</v>
@@ -748,6 +760,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="2"/>
+      <c r="E4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" t="s">
         <v>72</v>
@@ -764,6 +777,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="2"/>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -776,6 +790,7 @@
         <v>39</v>
       </c>
       <c r="D6" s="2"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -788,6 +803,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="2"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -800,6 +816,7 @@
         <v>43</v>
       </c>
       <c r="D8" s="2"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -812,6 +829,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="2"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -824,6 +842,7 @@
         <v>3</v>
       </c>
       <c r="D10" s="2"/>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -836,6 +855,7 @@
         <v>13</v>
       </c>
       <c r="D11" s="2"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -848,6 +868,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="2"/>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -859,7 +880,8 @@
       <c r="C13">
         <v>22</v>
       </c>
-      <c r="D13" s="3"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -871,7 +893,8 @@
       <c r="C14">
         <v>40</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -884,6 +907,7 @@
         <v>10</v>
       </c>
       <c r="D15" s="2"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -896,8 +920,9 @@
         <v>18</v>
       </c>
       <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -908,8 +933,9 @@
         <v>16</v>
       </c>
       <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -920,8 +946,9 @@
         <v>6</v>
       </c>
       <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -932,8 +959,9 @@
         <v>4</v>
       </c>
       <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -943,9 +971,10 @@
       <c r="C20">
         <v>37</v>
       </c>
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D20" s="2"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -956,8 +985,9 @@
         <v>8</v>
       </c>
       <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -968,8 +998,9 @@
         <v>11</v>
       </c>
       <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -980,8 +1011,9 @@
         <v>19</v>
       </c>
       <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -992,8 +1024,9 @@
         <v>2</v>
       </c>
       <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1004,8 +1037,9 @@
         <v>33</v>
       </c>
       <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1016,8 +1050,9 @@
         <v>17</v>
       </c>
       <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1028,8 +1063,9 @@
         <v>14</v>
       </c>
       <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1040,8 +1076,9 @@
         <v>16</v>
       </c>
       <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1052,8 +1089,9 @@
         <v>1</v>
       </c>
       <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1064,8 +1102,9 @@
         <v>25</v>
       </c>
       <c r="D30" s="2"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1076,8 +1115,9 @@
         <v>2</v>
       </c>
       <c r="D31" s="2"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1088,8 +1128,9 @@
         <v>7</v>
       </c>
       <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1100,8 +1141,9 @@
         <v>14</v>
       </c>
       <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1112,8 +1154,9 @@
         <v>21</v>
       </c>
       <c r="D34" s="2"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1124,8 +1167,9 @@
         <v>12</v>
       </c>
       <c r="D35" s="2"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1136,8 +1180,9 @@
         <v>1</v>
       </c>
       <c r="D36" s="2"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1148,8 +1193,9 @@
         <v>6</v>
       </c>
       <c r="D37" s="2"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1160,8 +1206,9 @@
         <v>2</v>
       </c>
       <c r="D38" s="2"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1172,8 +1219,9 @@
         <v>9</v>
       </c>
       <c r="D39" s="2"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1184,8 +1232,9 @@
         <v>18</v>
       </c>
       <c r="D40" s="2"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1196,8 +1245,9 @@
         <v>14</v>
       </c>
       <c r="D41" s="2"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1207,9 +1257,10 @@
       <c r="C42">
         <v>29</v>
       </c>
-      <c r="D42" s="3"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D42" s="2"/>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1219,9 +1270,10 @@
       <c r="C43">
         <v>46</v>
       </c>
-      <c r="D43" s="3"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D43" s="2"/>
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -1231,9 +1283,13 @@
       <c r="C44">
         <v>7</v>
       </c>
-      <c r="D44" s="3"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D44" s="2"/>
+      <c r="E44" s="3"/>
+      <c r="F44" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -1244,8 +1300,9 @@
         <v>2</v>
       </c>
       <c r="D45" s="2"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -1256,8 +1313,9 @@
         <v>13</v>
       </c>
       <c r="D46" s="2"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -1268,8 +1326,9 @@
         <v>12</v>
       </c>
       <c r="D47" s="2"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -1280,8 +1339,9 @@
         <v>1</v>
       </c>
       <c r="D48" s="2"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -1292,8 +1352,9 @@
         <v>24</v>
       </c>
       <c r="D49" s="2"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -1304,8 +1365,9 @@
         <v>2</v>
       </c>
       <c r="D50" s="2"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -1316,8 +1378,9 @@
         <v>6</v>
       </c>
       <c r="D51" s="2"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
@@ -1328,8 +1391,9 @@
         <v>2</v>
       </c>
       <c r="D52" s="2"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E52" s="3"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
@@ -1340,8 +1404,9 @@
         <v>20</v>
       </c>
       <c r="D53" s="2"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
@@ -1352,8 +1417,9 @@
         <v>7</v>
       </c>
       <c r="D54" s="2"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E54" s="3"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
@@ -1364,8 +1430,9 @@
         <v>1</v>
       </c>
       <c r="D55" s="2"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
@@ -1376,8 +1443,9 @@
         <v>2</v>
       </c>
       <c r="D56" s="2"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
@@ -1388,8 +1456,9 @@
         <v>7</v>
       </c>
       <c r="D57" s="2"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E57" s="3"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
@@ -1400,8 +1469,9 @@
         <v>3</v>
       </c>
       <c r="D58" s="2"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E58" s="3"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
@@ -1412,8 +1482,9 @@
         <v>4</v>
       </c>
       <c r="D59" s="2"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E59" s="3"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
@@ -1424,8 +1495,9 @@
         <v>6</v>
       </c>
       <c r="D60" s="2"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E60" s="3"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
@@ -1436,8 +1508,9 @@
         <v>2</v>
       </c>
       <c r="D61" s="2"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E61" s="3"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
@@ -1448,8 +1521,9 @@
         <v>2</v>
       </c>
       <c r="D62" s="2"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E62" s="3"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
@@ -1460,8 +1534,9 @@
         <v>1</v>
       </c>
       <c r="D63" s="2"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E63" s="3"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
@@ -1472,8 +1547,9 @@
         <v>11</v>
       </c>
       <c r="D64" s="2"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E64" s="3"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
@@ -1484,8 +1560,9 @@
         <v>4</v>
       </c>
       <c r="D65" s="2"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E65" s="3"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
@@ -1496,8 +1573,9 @@
         <v>6</v>
       </c>
       <c r="D66" s="2"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E66" s="3"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
@@ -1508,8 +1586,9 @@
         <v>35</v>
       </c>
       <c r="D67" s="2"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E67" s="3"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
@@ -1520,8 +1599,9 @@
         <v>4</v>
       </c>
       <c r="D68" s="2"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E68" s="3"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
@@ -1532,8 +1612,12 @@
         <v>25</v>
       </c>
       <c r="D69" s="2"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E69" s="3"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>68</v>
+      </c>
       <c r="B70" t="s">
         <v>69</v>
       </c>
@@ -1541,6 +1625,7 @@
         <v>18</v>
       </c>
       <c r="D70" s="2"/>
+      <c r="E70" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added code to some src scripts and closed issues
</commit_message>
<xml_diff>
--- a/Docs/HistoryScrapeStatus.xlsx
+++ b/Docs/HistoryScrapeStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpete\Documents\Projects\CarStats\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D838CD7-4541-466E-9BA2-669EE6F9E5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DBF9A3-C506-4E2B-9B80-CF2B29CE5528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-3945" windowWidth="29040" windowHeight="15840" xr2:uid="{84160147-604C-44EB-89D6-C5A3DE91A955}"/>
   </bookViews>
@@ -679,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2B1DA9D-AC09-4F91-8BA6-4CCF32CADB06}">
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="K58" sqref="K58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1414,7 +1414,7 @@
         <v>53</v>
       </c>
       <c r="C54">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="3"/>

</xml_diff>

<commit_message>
More corrections scripts. About 2/3 way done for model corrections
</commit_message>
<xml_diff>
--- a/Docs/HistoryScrapeStatus.xlsx
+++ b/Docs/HistoryScrapeStatus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpete\Documents\Projects\CarStats\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DBF9A3-C506-4E2B-9B80-CF2B29CE5528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBB1A7A-E3DC-4071-BD0A-21305171AF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-3945" windowWidth="29040" windowHeight="15840" xr2:uid="{84160147-604C-44EB-89D6-C5A3DE91A955}"/>
+    <workbookView xWindow="-28920" yWindow="-3795" windowWidth="29040" windowHeight="15840" xr2:uid="{84160147-604C-44EB-89D6-C5A3DE91A955}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -354,12 +354,20 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -677,955 +685,893 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2B1DA9D-AC09-4F91-8BA6-4CCF32CADB06}">
-  <dimension ref="A1:J70"/>
+  <dimension ref="A1:L70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>74</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="4">
+        <v>2023</v>
+      </c>
+      <c r="F1" s="4">
+        <v>2024</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="6">
         <v>11</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="I2" s="2"/>
-      <c r="J2" t="s">
+      <c r="K2" s="2"/>
+      <c r="L2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>75</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="6">
         <v>1</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="I3" s="1"/>
-      <c r="J3" t="s">
+      <c r="K3" s="1"/>
+      <c r="L3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="6">
         <v>8</v>
       </c>
       <c r="D4" s="2"/>
-      <c r="E4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" t="s">
+      <c r="K4" s="3"/>
+      <c r="L4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="6">
         <v>11</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="6">
         <v>39</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="6">
         <v>9</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="6">
         <v>43</v>
       </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="6">
         <v>2</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="6">
         <v>3</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="6">
         <v>13</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="6">
         <v>1</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="6">
         <v>22</v>
       </c>
       <c r="D13" s="2"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="6">
         <v>40</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="6">
         <v>10</v>
       </c>
       <c r="D15" s="2"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="6">
         <v>18</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="6">
         <v>16</v>
       </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="6">
         <v>6</v>
       </c>
       <c r="D18" s="2"/>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="6">
         <v>4</v>
       </c>
       <c r="D19" s="2"/>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="6">
         <v>37</v>
       </c>
       <c r="D20" s="2"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="6">
         <v>8</v>
       </c>
       <c r="D21" s="2"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="6">
         <v>11</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="6">
         <v>19</v>
       </c>
       <c r="D23" s="2"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="6">
         <v>2</v>
       </c>
       <c r="D24" s="2"/>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="6">
         <v>33</v>
       </c>
       <c r="D25" s="2"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="6">
         <v>17</v>
       </c>
       <c r="D26" s="2"/>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="6">
         <v>14</v>
       </c>
       <c r="D27" s="2"/>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="6">
         <v>16</v>
       </c>
       <c r="D28" s="2"/>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>28</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="6">
         <v>1</v>
       </c>
       <c r="D29" s="2"/>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="6">
         <v>25</v>
       </c>
       <c r="D30" s="2"/>
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="6">
         <v>2</v>
       </c>
       <c r="D31" s="2"/>
-      <c r="E31" s="3"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32" t="s">
         <v>31</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="6">
         <v>7</v>
       </c>
       <c r="D32" s="2"/>
-      <c r="E32" s="3"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33" t="s">
         <v>32</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="6">
         <v>14</v>
       </c>
       <c r="D33" s="2"/>
-      <c r="E33" s="3"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34" t="s">
         <v>33</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="6">
         <v>21</v>
       </c>
       <c r="D34" s="2"/>
-      <c r="E34" s="3"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35" t="s">
         <v>34</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="6">
         <v>12</v>
       </c>
       <c r="D35" s="2"/>
-      <c r="E35" s="3"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>35</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="6">
         <v>1</v>
       </c>
       <c r="D36" s="2"/>
-      <c r="E36" s="3"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37" t="s">
         <v>36</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="6">
         <v>6</v>
       </c>
       <c r="D37" s="2"/>
-      <c r="E37" s="3"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38" t="s">
         <v>37</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="6">
         <v>2</v>
       </c>
       <c r="D38" s="2"/>
-      <c r="E38" s="3"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39" t="s">
         <v>38</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="6">
         <v>9</v>
       </c>
       <c r="D39" s="2"/>
-      <c r="E39" s="3"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40" t="s">
         <v>39</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="6">
         <v>18</v>
       </c>
       <c r="D40" s="2"/>
-      <c r="E40" s="3"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41" t="s">
         <v>40</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="6">
         <v>14</v>
       </c>
       <c r="D41" s="2"/>
-      <c r="E41" s="3"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42" t="s">
         <v>41</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="6">
         <v>29</v>
       </c>
       <c r="D42" s="2"/>
-      <c r="E42" s="3"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="B43" t="s">
         <v>42</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="6">
         <v>46</v>
       </c>
       <c r="D43" s="2"/>
-      <c r="E43" s="3"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
       <c r="B44" t="s">
         <v>43</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="6">
         <v>7</v>
       </c>
       <c r="D44" s="2"/>
-      <c r="E44" s="3"/>
-      <c r="F44" t="s">
+      <c r="H44" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45" t="s">
         <v>44</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="6">
         <v>2</v>
       </c>
       <c r="D45" s="2"/>
-      <c r="E45" s="3"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="B46" t="s">
         <v>45</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="6">
         <v>13</v>
       </c>
       <c r="D46" s="2"/>
-      <c r="E46" s="3"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="B47" t="s">
         <v>46</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="6">
         <v>12</v>
       </c>
       <c r="D47" s="2"/>
-      <c r="E47" s="3"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
       <c r="B48" t="s">
         <v>47</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="6">
         <v>1</v>
       </c>
       <c r="D48" s="2"/>
-      <c r="E48" s="3"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
       <c r="B49" t="s">
         <v>48</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="6">
         <v>24</v>
       </c>
       <c r="D49" s="2"/>
-      <c r="E49" s="3"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
       <c r="B50" t="s">
         <v>49</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="6">
         <v>2</v>
       </c>
       <c r="D50" s="2"/>
-      <c r="E50" s="3"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
       <c r="B51" t="s">
         <v>50</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="6">
         <v>6</v>
       </c>
       <c r="D51" s="2"/>
-      <c r="E51" s="3"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
       <c r="B52" t="s">
         <v>51</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="6">
         <v>2</v>
       </c>
       <c r="D52" s="2"/>
-      <c r="E52" s="3"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
       <c r="B53" t="s">
         <v>52</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="6">
         <v>20</v>
       </c>
       <c r="D53" s="2"/>
-      <c r="E53" s="3"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
       <c r="B54" t="s">
         <v>53</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="6">
         <v>6</v>
       </c>
       <c r="D54" s="2"/>
-      <c r="E54" s="3"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
       <c r="B55" t="s">
         <v>54</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="6">
         <v>1</v>
       </c>
       <c r="D55" s="2"/>
-      <c r="E55" s="3"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
       <c r="B56" t="s">
         <v>55</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="6">
         <v>2</v>
       </c>
       <c r="D56" s="2"/>
-      <c r="E56" s="3"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
       <c r="B57" t="s">
         <v>56</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="6">
         <v>7</v>
       </c>
       <c r="D57" s="2"/>
-      <c r="E57" s="3"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
       <c r="B58" t="s">
         <v>57</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="6">
         <v>3</v>
       </c>
       <c r="D58" s="2"/>
-      <c r="E58" s="3"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
       <c r="B59" t="s">
         <v>58</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="6">
         <v>4</v>
       </c>
       <c r="D59" s="2"/>
-      <c r="E59" s="3"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
       <c r="B60" t="s">
         <v>59</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="6">
         <v>6</v>
       </c>
       <c r="D60" s="2"/>
-      <c r="E60" s="3"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
       <c r="B61" t="s">
         <v>60</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="6">
         <v>2</v>
       </c>
       <c r="D61" s="2"/>
-      <c r="E61" s="3"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
       <c r="B62" t="s">
         <v>61</v>
       </c>
-      <c r="C62">
+      <c r="C62" s="6">
         <v>2</v>
       </c>
       <c r="D62" s="2"/>
-      <c r="E62" s="3"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
       <c r="B63" t="s">
         <v>62</v>
       </c>
-      <c r="C63">
+      <c r="C63" s="6">
         <v>1</v>
       </c>
       <c r="D63" s="2"/>
-      <c r="E63" s="3"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
       <c r="B64" t="s">
         <v>63</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="6">
         <v>11</v>
       </c>
       <c r="D64" s="2"/>
-      <c r="E64" s="3"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
       <c r="B65" t="s">
         <v>64</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="6">
         <v>4</v>
       </c>
       <c r="D65" s="2"/>
-      <c r="E65" s="3"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
       <c r="B66" t="s">
         <v>65</v>
       </c>
-      <c r="C66">
+      <c r="C66" s="6">
         <v>6</v>
       </c>
       <c r="D66" s="2"/>
-      <c r="E66" s="3"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
       <c r="B67" t="s">
         <v>66</v>
       </c>
-      <c r="C67">
+      <c r="C67" s="6">
         <v>35</v>
       </c>
       <c r="D67" s="2"/>
-      <c r="E67" s="3"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
       <c r="B68" t="s">
         <v>67</v>
       </c>
-      <c r="C68">
+      <c r="C68" s="6">
         <v>4</v>
       </c>
       <c r="D68" s="2"/>
-      <c r="E68" s="3"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
       <c r="B69" t="s">
         <v>68</v>
       </c>
-      <c r="C69">
+      <c r="C69" s="6">
         <v>25</v>
       </c>
       <c r="D69" s="2"/>
-      <c r="E69" s="3"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>68</v>
       </c>
       <c r="B70" t="s">
         <v>69</v>
       </c>
-      <c r="C70">
+      <c r="C70" s="6">
         <v>18</v>
       </c>
       <c r="D70" s="2"/>
-      <c r="E70" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Scraper 2.0 just about done
</commit_message>
<xml_diff>
--- a/Docs/HistoryScrapeStatus.xlsx
+++ b/Docs/HistoryScrapeStatus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpete\Documents\Projects\CarStats\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBB1A7A-E3DC-4071-BD0A-21305171AF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434D35B4-73BA-48BE-A93E-B8D67AFA73A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3795" windowWidth="29040" windowHeight="15840" xr2:uid="{84160147-604C-44EB-89D6-C5A3DE91A955}"/>
+    <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="15840" xr2:uid="{84160147-604C-44EB-89D6-C5A3DE91A955}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>Index</t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>Buggy links all over the place</t>
+  </si>
+  <si>
+    <t>History Status v2.0</t>
   </si>
 </sst>
 </file>
@@ -354,7 +357,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -368,6 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -688,7 +692,7 @@
   <dimension ref="A1:L70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -696,8 +700,9 @@
     <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
@@ -717,8 +722,8 @@
       <c r="D1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="4">
-        <v>2023</v>
+      <c r="E1" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="F1" s="4">
         <v>2024</v>
@@ -740,7 +745,7 @@
       <c r="C2" s="6">
         <v>11</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="7"/>
       <c r="K2" s="2"/>
       <c r="L2" t="s">
         <v>76</v>
@@ -756,7 +761,7 @@
       <c r="C3" s="6">
         <v>1</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="7"/>
       <c r="K3" s="1"/>
       <c r="L3" t="s">
         <v>71</v>
@@ -772,7 +777,7 @@
       <c r="C4" s="6">
         <v>8</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="7"/>
       <c r="K4" s="3"/>
       <c r="L4" t="s">
         <v>72</v>
@@ -788,7 +793,7 @@
       <c r="C5" s="6">
         <v>11</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="7"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -800,7 +805,7 @@
       <c r="C6" s="6">
         <v>39</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -812,7 +817,7 @@
       <c r="C7" s="6">
         <v>9</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -824,7 +829,7 @@
       <c r="C8" s="6">
         <v>43</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -836,7 +841,7 @@
       <c r="C9" s="6">
         <v>2</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="7"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -848,7 +853,7 @@
       <c r="C10" s="6">
         <v>3</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -860,7 +865,7 @@
       <c r="C11" s="6">
         <v>13</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="7"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -872,7 +877,7 @@
       <c r="C12" s="6">
         <v>1</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="7"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -884,7 +889,7 @@
       <c r="C13" s="6">
         <v>22</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -896,7 +901,7 @@
       <c r="C14" s="6">
         <v>40</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -908,7 +913,7 @@
       <c r="C15" s="6">
         <v>10</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -920,7 +925,7 @@
       <c r="C16" s="6">
         <v>18</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="7"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
@@ -932,7 +937,7 @@
       <c r="C17" s="6">
         <v>16</v>
       </c>
-      <c r="D17" s="2"/>
+      <c r="D17" s="7"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
@@ -944,7 +949,7 @@
       <c r="C18" s="6">
         <v>6</v>
       </c>
-      <c r="D18" s="2"/>
+      <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
@@ -956,7 +961,7 @@
       <c r="C19" s="6">
         <v>4</v>
       </c>
-      <c r="D19" s="2"/>
+      <c r="D19" s="7"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
@@ -968,7 +973,7 @@
       <c r="C20" s="6">
         <v>37</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
@@ -980,7 +985,7 @@
       <c r="C21" s="6">
         <v>8</v>
       </c>
-      <c r="D21" s="2"/>
+      <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
@@ -992,7 +997,7 @@
       <c r="C22" s="6">
         <v>11</v>
       </c>
-      <c r="D22" s="2"/>
+      <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
@@ -1004,7 +1009,7 @@
       <c r="C23" s="6">
         <v>19</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
@@ -1016,7 +1021,7 @@
       <c r="C24" s="6">
         <v>2</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
@@ -1028,7 +1033,7 @@
       <c r="C25" s="6">
         <v>33</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
@@ -1040,7 +1045,7 @@
       <c r="C26" s="6">
         <v>17</v>
       </c>
-      <c r="D26" s="2"/>
+      <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
@@ -1052,7 +1057,7 @@
       <c r="C27" s="6">
         <v>14</v>
       </c>
-      <c r="D27" s="2"/>
+      <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
@@ -1064,7 +1069,7 @@
       <c r="C28" s="6">
         <v>16</v>
       </c>
-      <c r="D28" s="2"/>
+      <c r="D28" s="7"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
@@ -1076,7 +1081,7 @@
       <c r="C29" s="6">
         <v>1</v>
       </c>
-      <c r="D29" s="2"/>
+      <c r="D29" s="7"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
@@ -1088,7 +1093,7 @@
       <c r="C30" s="6">
         <v>25</v>
       </c>
-      <c r="D30" s="2"/>
+      <c r="D30" s="7"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
@@ -1100,7 +1105,7 @@
       <c r="C31" s="6">
         <v>2</v>
       </c>
-      <c r="D31" s="2"/>
+      <c r="D31" s="7"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
@@ -1112,7 +1117,7 @@
       <c r="C32" s="6">
         <v>7</v>
       </c>
-      <c r="D32" s="2"/>
+      <c r="D32" s="7"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
@@ -1124,7 +1129,7 @@
       <c r="C33" s="6">
         <v>14</v>
       </c>
-      <c r="D33" s="2"/>
+      <c r="D33" s="7"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
@@ -1136,7 +1141,7 @@
       <c r="C34" s="6">
         <v>21</v>
       </c>
-      <c r="D34" s="2"/>
+      <c r="D34" s="7"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
@@ -1148,7 +1153,7 @@
       <c r="C35" s="6">
         <v>12</v>
       </c>
-      <c r="D35" s="2"/>
+      <c r="D35" s="7"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
@@ -1160,7 +1165,7 @@
       <c r="C36" s="6">
         <v>1</v>
       </c>
-      <c r="D36" s="2"/>
+      <c r="D36" s="7"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
@@ -1172,7 +1177,7 @@
       <c r="C37" s="6">
         <v>6</v>
       </c>
-      <c r="D37" s="2"/>
+      <c r="D37" s="7"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
@@ -1184,7 +1189,7 @@
       <c r="C38" s="6">
         <v>2</v>
       </c>
-      <c r="D38" s="2"/>
+      <c r="D38" s="7"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
@@ -1196,7 +1201,7 @@
       <c r="C39" s="6">
         <v>9</v>
       </c>
-      <c r="D39" s="2"/>
+      <c r="D39" s="7"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
@@ -1208,7 +1213,7 @@
       <c r="C40" s="6">
         <v>18</v>
       </c>
-      <c r="D40" s="2"/>
+      <c r="D40" s="7"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
@@ -1220,7 +1225,7 @@
       <c r="C41" s="6">
         <v>14</v>
       </c>
-      <c r="D41" s="2"/>
+      <c r="D41" s="7"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
@@ -1232,7 +1237,7 @@
       <c r="C42" s="6">
         <v>29</v>
       </c>
-      <c r="D42" s="2"/>
+      <c r="D42" s="7"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
@@ -1244,7 +1249,7 @@
       <c r="C43" s="6">
         <v>46</v>
       </c>
-      <c r="D43" s="2"/>
+      <c r="D43" s="7"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
@@ -1256,7 +1261,7 @@
       <c r="C44" s="6">
         <v>7</v>
       </c>
-      <c r="D44" s="2"/>
+      <c r="D44" s="7"/>
       <c r="H44" t="s">
         <v>78</v>
       </c>
@@ -1271,7 +1276,7 @@
       <c r="C45" s="6">
         <v>2</v>
       </c>
-      <c r="D45" s="2"/>
+      <c r="D45" s="7"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
@@ -1283,7 +1288,7 @@
       <c r="C46" s="6">
         <v>13</v>
       </c>
-      <c r="D46" s="2"/>
+      <c r="D46" s="7"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
@@ -1295,7 +1300,7 @@
       <c r="C47" s="6">
         <v>12</v>
       </c>
-      <c r="D47" s="2"/>
+      <c r="D47" s="7"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
@@ -1307,7 +1312,7 @@
       <c r="C48" s="6">
         <v>1</v>
       </c>
-      <c r="D48" s="2"/>
+      <c r="D48" s="7"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
@@ -1319,7 +1324,7 @@
       <c r="C49" s="6">
         <v>24</v>
       </c>
-      <c r="D49" s="2"/>
+      <c r="D49" s="7"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
@@ -1331,7 +1336,7 @@
       <c r="C50" s="6">
         <v>2</v>
       </c>
-      <c r="D50" s="2"/>
+      <c r="D50" s="7"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
@@ -1343,7 +1348,7 @@
       <c r="C51" s="6">
         <v>6</v>
       </c>
-      <c r="D51" s="2"/>
+      <c r="D51" s="7"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
@@ -1355,7 +1360,7 @@
       <c r="C52" s="6">
         <v>2</v>
       </c>
-      <c r="D52" s="2"/>
+      <c r="D52" s="7"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
@@ -1367,7 +1372,7 @@
       <c r="C53" s="6">
         <v>20</v>
       </c>
-      <c r="D53" s="2"/>
+      <c r="D53" s="7"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
@@ -1379,7 +1384,7 @@
       <c r="C54" s="6">
         <v>6</v>
       </c>
-      <c r="D54" s="2"/>
+      <c r="D54" s="7"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
@@ -1391,7 +1396,7 @@
       <c r="C55" s="6">
         <v>1</v>
       </c>
-      <c r="D55" s="2"/>
+      <c r="D55" s="7"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
@@ -1403,7 +1408,7 @@
       <c r="C56" s="6">
         <v>2</v>
       </c>
-      <c r="D56" s="2"/>
+      <c r="D56" s="7"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
@@ -1415,7 +1420,7 @@
       <c r="C57" s="6">
         <v>7</v>
       </c>
-      <c r="D57" s="2"/>
+      <c r="D57" s="7"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
@@ -1427,7 +1432,7 @@
       <c r="C58" s="6">
         <v>3</v>
       </c>
-      <c r="D58" s="2"/>
+      <c r="D58" s="7"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
@@ -1439,7 +1444,7 @@
       <c r="C59" s="6">
         <v>4</v>
       </c>
-      <c r="D59" s="2"/>
+      <c r="D59" s="7"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
@@ -1451,7 +1456,7 @@
       <c r="C60" s="6">
         <v>6</v>
       </c>
-      <c r="D60" s="2"/>
+      <c r="D60" s="7"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
@@ -1463,7 +1468,7 @@
       <c r="C61" s="6">
         <v>2</v>
       </c>
-      <c r="D61" s="2"/>
+      <c r="D61" s="7"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
@@ -1475,7 +1480,7 @@
       <c r="C62" s="6">
         <v>2</v>
       </c>
-      <c r="D62" s="2"/>
+      <c r="D62" s="7"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
@@ -1487,7 +1492,7 @@
       <c r="C63" s="6">
         <v>1</v>
       </c>
-      <c r="D63" s="2"/>
+      <c r="D63" s="7"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
@@ -1499,9 +1504,9 @@
       <c r="C64" s="6">
         <v>11</v>
       </c>
-      <c r="D64" s="2"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D64" s="7"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
@@ -1511,9 +1516,9 @@
       <c r="C65" s="6">
         <v>4</v>
       </c>
-      <c r="D65" s="2"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D65" s="7"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
@@ -1523,9 +1528,10 @@
       <c r="C66" s="6">
         <v>6</v>
       </c>
-      <c r="D66" s="2"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D66" s="7"/>
+      <c r="E66" s="2"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
@@ -1535,9 +1541,9 @@
       <c r="C67" s="6">
         <v>35</v>
       </c>
-      <c r="D67" s="2"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D67" s="7"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
@@ -1547,9 +1553,9 @@
       <c r="C68" s="6">
         <v>4</v>
       </c>
-      <c r="D68" s="2"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D68" s="7"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
@@ -1559,9 +1565,9 @@
       <c r="C69" s="6">
         <v>25</v>
       </c>
-      <c r="D69" s="2"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D69" s="7"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>68</v>
       </c>
@@ -1571,7 +1577,7 @@
       <c r="C70" s="6">
         <v>18</v>
       </c>
-      <c r="D70" s="2"/>
+      <c r="D70" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
More work, but major bug in scraper now that UI chanced, this needs to be fixed
</commit_message>
<xml_diff>
--- a/Docs/HistoryScrapeStatus.xlsx
+++ b/Docs/HistoryScrapeStatus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpete\Documents\Projects\CarStats\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434D35B4-73BA-48BE-A93E-B8D67AFA73A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8153AB83-B7F8-4D38-91A0-01E72E3D7C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="15840" xr2:uid="{84160147-604C-44EB-89D6-C5A3DE91A955}"/>
+    <workbookView xWindow="-28920" yWindow="-3435" windowWidth="29040" windowHeight="15840" xr2:uid="{84160147-604C-44EB-89D6-C5A3DE91A955}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>Index</t>
   </si>
@@ -267,12 +267,6 @@
   </si>
   <si>
     <t>Done</t>
-  </si>
-  <si>
-    <t>Error Link Handling</t>
-  </si>
-  <si>
-    <t>Buggy links all over the place</t>
   </si>
   <si>
     <t>History Status v2.0</t>
@@ -692,7 +686,7 @@
   <dimension ref="A1:L70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -723,13 +717,10 @@
         <v>73</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F1" s="4">
         <v>2024</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>70</v>
@@ -746,6 +737,7 @@
         <v>11</v>
       </c>
       <c r="D2" s="7"/>
+      <c r="E2" s="1"/>
       <c r="K2" s="2"/>
       <c r="L2" t="s">
         <v>76</v>
@@ -762,6 +754,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="7"/>
+      <c r="E3" s="3"/>
       <c r="K3" s="1"/>
       <c r="L3" t="s">
         <v>71</v>
@@ -775,9 +768,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="7"/>
+      <c r="E4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" t="s">
         <v>72</v>
@@ -791,9 +785,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="6">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="7"/>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -803,9 +798,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="6">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D6" s="7"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -818,6 +814,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="7"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -830,6 +827,7 @@
         <v>43</v>
       </c>
       <c r="D8" s="7"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -842,6 +840,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="7"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -854,6 +853,7 @@
         <v>3</v>
       </c>
       <c r="D10" s="7"/>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -866,6 +866,7 @@
         <v>13</v>
       </c>
       <c r="D11" s="7"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -878,6 +879,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="7"/>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -887,9 +889,10 @@
         <v>12</v>
       </c>
       <c r="C13" s="6">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D13" s="7"/>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -902,6 +905,7 @@
         <v>40</v>
       </c>
       <c r="D14" s="7"/>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -914,6 +918,7 @@
         <v>10</v>
       </c>
       <c r="D15" s="7"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -923,11 +928,12 @@
         <v>15</v>
       </c>
       <c r="C16" s="6">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" s="7"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -938,8 +944,9 @@
         <v>16</v>
       </c>
       <c r="D17" s="7"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -950,8 +957,9 @@
         <v>6</v>
       </c>
       <c r="D18" s="7"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -959,11 +967,12 @@
         <v>18</v>
       </c>
       <c r="C19" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D19" s="7"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -971,11 +980,12 @@
         <v>19</v>
       </c>
       <c r="C20" s="6">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D20" s="7"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -983,11 +993,12 @@
         <v>20</v>
       </c>
       <c r="C21" s="6">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D21" s="7"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -998,8 +1009,9 @@
         <v>11</v>
       </c>
       <c r="D22" s="7"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1010,8 +1022,9 @@
         <v>19</v>
       </c>
       <c r="D23" s="7"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1022,8 +1035,9 @@
         <v>2</v>
       </c>
       <c r="D24" s="7"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1031,11 +1045,12 @@
         <v>24</v>
       </c>
       <c r="C25" s="6">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D25" s="7"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1043,11 +1058,12 @@
         <v>25</v>
       </c>
       <c r="C26" s="6">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D26" s="7"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1058,8 +1074,9 @@
         <v>14</v>
       </c>
       <c r="D27" s="7"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1070,8 +1087,9 @@
         <v>16</v>
       </c>
       <c r="D28" s="7"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1082,8 +1100,9 @@
         <v>1</v>
       </c>
       <c r="D29" s="7"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1091,11 +1110,12 @@
         <v>29</v>
       </c>
       <c r="C30" s="6">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D30" s="7"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1106,8 +1126,9 @@
         <v>2</v>
       </c>
       <c r="D31" s="7"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1115,11 +1136,12 @@
         <v>31</v>
       </c>
       <c r="C32" s="6">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D32" s="7"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1130,8 +1152,9 @@
         <v>14</v>
       </c>
       <c r="D33" s="7"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1139,11 +1162,12 @@
         <v>33</v>
       </c>
       <c r="C34" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D34" s="7"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1154,8 +1178,9 @@
         <v>12</v>
       </c>
       <c r="D35" s="7"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1166,8 +1191,9 @@
         <v>1</v>
       </c>
       <c r="D36" s="7"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1175,11 +1201,12 @@
         <v>36</v>
       </c>
       <c r="C37" s="6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D37" s="7"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1190,8 +1217,9 @@
         <v>2</v>
       </c>
       <c r="D38" s="7"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1202,8 +1230,9 @@
         <v>9</v>
       </c>
       <c r="D39" s="7"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1214,8 +1243,9 @@
         <v>18</v>
       </c>
       <c r="D40" s="7"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1226,8 +1256,9 @@
         <v>14</v>
       </c>
       <c r="D41" s="7"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1235,11 +1266,12 @@
         <v>41</v>
       </c>
       <c r="C42" s="6">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D42" s="7"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1247,11 +1279,12 @@
         <v>42</v>
       </c>
       <c r="C43" s="6">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D43" s="7"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -1262,11 +1295,9 @@
         <v>7</v>
       </c>
       <c r="D44" s="7"/>
-      <c r="H44" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -1274,11 +1305,12 @@
         <v>44</v>
       </c>
       <c r="C45" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D45" s="7"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -1286,11 +1318,12 @@
         <v>45</v>
       </c>
       <c r="C46" s="6">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D46" s="7"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -1301,8 +1334,9 @@
         <v>12</v>
       </c>
       <c r="D47" s="7"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -1313,8 +1347,9 @@
         <v>1</v>
       </c>
       <c r="D48" s="7"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -1325,8 +1360,9 @@
         <v>24</v>
       </c>
       <c r="D49" s="7"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -1337,8 +1373,9 @@
         <v>2</v>
       </c>
       <c r="D50" s="7"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -1349,8 +1386,9 @@
         <v>6</v>
       </c>
       <c r="D51" s="7"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
@@ -1361,8 +1399,9 @@
         <v>2</v>
       </c>
       <c r="D52" s="7"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E52" s="3"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
@@ -1370,11 +1409,12 @@
         <v>52</v>
       </c>
       <c r="C53" s="6">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D53" s="7"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
@@ -1382,11 +1422,12 @@
         <v>53</v>
       </c>
       <c r="C54" s="6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D54" s="7"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E54" s="3"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
@@ -1397,8 +1438,9 @@
         <v>1</v>
       </c>
       <c r="D55" s="7"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
@@ -1406,11 +1448,12 @@
         <v>55</v>
       </c>
       <c r="C56" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D56" s="7"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
@@ -1421,8 +1464,9 @@
         <v>7</v>
       </c>
       <c r="D57" s="7"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E57" s="3"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
@@ -1433,8 +1477,9 @@
         <v>3</v>
       </c>
       <c r="D58" s="7"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E58" s="3"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
@@ -1445,8 +1490,9 @@
         <v>4</v>
       </c>
       <c r="D59" s="7"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E59" s="3"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
@@ -1457,8 +1503,9 @@
         <v>6</v>
       </c>
       <c r="D60" s="7"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E60" s="3"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
@@ -1469,8 +1516,9 @@
         <v>2</v>
       </c>
       <c r="D61" s="7"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E61" s="3"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
@@ -1481,8 +1529,9 @@
         <v>2</v>
       </c>
       <c r="D62" s="7"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E62" s="3"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
@@ -1493,8 +1542,9 @@
         <v>1</v>
       </c>
       <c r="D63" s="7"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E63" s="3"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
@@ -1505,6 +1555,7 @@
         <v>11</v>
       </c>
       <c r="D64" s="7"/>
+      <c r="E64" s="3"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65">
@@ -1517,6 +1568,7 @@
         <v>4</v>
       </c>
       <c r="D65" s="7"/>
+      <c r="E65" s="3"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66">
@@ -1539,9 +1591,10 @@
         <v>66</v>
       </c>
       <c r="C67" s="6">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D67" s="7"/>
+      <c r="E67" s="3"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68">
@@ -1554,6 +1607,7 @@
         <v>4</v>
       </c>
       <c r="D68" s="7"/>
+      <c r="E68" s="3"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69">
@@ -1566,6 +1620,7 @@
         <v>25</v>
       </c>
       <c r="D69" s="7"/>
+      <c r="E69" s="3"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70">
@@ -1575,9 +1630,10 @@
         <v>69</v>
       </c>
       <c r="C70" s="6">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D70" s="7"/>
+      <c r="E70" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed scraper for new UI, still a few kinks to work out, longer sleep constant is more robust but takes longer... running full scrape again, see HistoryScrapeStatus.xlsx for progress details
</commit_message>
<xml_diff>
--- a/Docs/HistoryScrapeStatus.xlsx
+++ b/Docs/HistoryScrapeStatus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpete\Documents\Projects\CarStats\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8153AB83-B7F8-4D38-91A0-01E72E3D7C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B0494C-4B5B-41F6-89DF-0B2D1B0391FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3435" windowWidth="29040" windowHeight="15840" xr2:uid="{84160147-604C-44EB-89D6-C5A3DE91A955}"/>
+    <workbookView xWindow="-57720" yWindow="-3435" windowWidth="29040" windowHeight="15840" xr2:uid="{84160147-604C-44EB-89D6-C5A3DE91A955}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -686,7 +686,7 @@
   <dimension ref="A1:L70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -737,7 +737,7 @@
         <v>11</v>
       </c>
       <c r="D2" s="7"/>
-      <c r="E2" s="1"/>
+      <c r="E2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" t="s">
         <v>76</v>
@@ -754,7 +754,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="7"/>
-      <c r="E3" s="3"/>
+      <c r="E3" s="2"/>
       <c r="K3" s="1"/>
       <c r="L3" t="s">
         <v>71</v>
@@ -771,7 +771,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="7"/>
-      <c r="E4" s="3"/>
+      <c r="E4" s="2"/>
       <c r="K4" s="3"/>
       <c r="L4" t="s">
         <v>72</v>
@@ -788,7 +788,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="7"/>
-      <c r="E5" s="3"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">

</xml_diff>

<commit_message>
More fixes and progress in scraping data
</commit_message>
<xml_diff>
--- a/Docs/HistoryScrapeStatus.xlsx
+++ b/Docs/HistoryScrapeStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpete\Documents\Projects\CarStats\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B0494C-4B5B-41F6-89DF-0B2D1B0391FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3AE5B4-3F13-4930-A281-0E712B051C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-3435" windowWidth="29040" windowHeight="15840" xr2:uid="{84160147-604C-44EB-89D6-C5A3DE91A955}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>Index</t>
   </si>
@@ -260,9 +260,6 @@
     <t>History Status</t>
   </si>
   <si>
-    <t>Size (links)</t>
-  </si>
-  <si>
     <t>Afeela</t>
   </si>
   <si>
@@ -270,13 +267,22 @@
   </si>
   <si>
     <t>History Status v2.0</t>
+  </si>
+  <si>
+    <t>Completion</t>
+  </si>
+  <si>
+    <t>Size (base links)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000%"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,6 +312,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -345,13 +366,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -359,19 +381,31 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
+    <cellStyle name="Good" xfId="1" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="4" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -683,19 +717,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2B1DA9D-AC09-4F91-8BA6-4CCF32CADB06}">
-  <dimension ref="A1:L70"/>
+  <dimension ref="A1:L72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
-    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="5" max="5" width="19.77734375" style="6" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4.21875" bestFit="1" customWidth="1"/>
@@ -704,936 +738,978 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="4">
-        <v>2024</v>
-      </c>
-      <c r="K1" s="4" t="s">
+      <c r="E1" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="5">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>11</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="2"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="9">
+        <v>11</v>
+      </c>
       <c r="K2" s="2"/>
       <c r="L2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="6">
+        <v>74</v>
+      </c>
+      <c r="C3" s="5">
         <v>1</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="2"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="9">
+        <v>1</v>
+      </c>
       <c r="K3" s="1"/>
       <c r="L3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>9</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="2"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="9">
+        <v>9</v>
+      </c>
       <c r="K4" s="3"/>
       <c r="L4" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>12</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="2"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="9">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>40</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="3"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="9">
+        <v>40</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>9</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="3"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="9">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>43</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="3"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="9">
+        <v>43</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="5">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>2</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="3"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="5">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>3</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="3"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="5">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>13</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="3"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="9">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="5">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>1</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="3"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="5">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>23</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="3"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="10"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="5">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>40</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="3"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="5">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>10</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="3"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="5">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <v>17</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="3"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="10"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="A17" s="5">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>16</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="3"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="10"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" s="5">
         <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="5">
         <v>6</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="3"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="A19" s="5">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>5</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="3"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="10"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="A20" s="5">
         <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <v>39</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="3"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="10"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="A21" s="5">
         <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="5">
         <v>11</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="3"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="10"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22">
+      <c r="A22" s="5">
         <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="5">
         <v>11</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="3"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="10"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23">
+      <c r="A23" s="5">
         <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="5">
         <v>19</v>
       </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="3"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="10"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24">
+      <c r="A24" s="5">
         <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="5">
         <v>2</v>
       </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="3"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="10"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25">
+      <c r="A25" s="5">
         <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="5">
         <v>36</v>
       </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="3"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="10"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26">
+      <c r="A26" s="5">
         <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="5">
         <v>16</v>
       </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="3"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="10"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27">
+      <c r="A27" s="5">
         <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="5">
         <v>14</v>
       </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="3"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="10"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28">
+      <c r="A28" s="5">
         <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="5">
         <v>16</v>
       </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="3"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="10"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29">
+      <c r="A29" s="5">
         <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="5">
         <v>1</v>
       </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="3"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="10"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30">
+      <c r="A30" s="5">
         <v>28</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="5">
         <v>27</v>
       </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="3"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="10"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31">
+      <c r="A31" s="5">
         <v>29</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="5">
         <v>2</v>
       </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="3"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="10"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32">
+      <c r="A32" s="5">
         <v>30</v>
       </c>
       <c r="B32" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="5">
         <v>9</v>
       </c>
-      <c r="D32" s="7"/>
-      <c r="E32" s="3"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="10"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33">
+      <c r="A33" s="5">
         <v>31</v>
       </c>
       <c r="B33" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" s="5">
         <v>14</v>
       </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="3"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="10"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34">
+      <c r="A34" s="5">
         <v>32</v>
       </c>
       <c r="B34" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="5">
         <v>22</v>
       </c>
-      <c r="D34" s="7"/>
-      <c r="E34" s="3"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="10"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35">
+      <c r="A35" s="5">
         <v>33</v>
       </c>
       <c r="B35" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" s="5">
         <v>12</v>
       </c>
-      <c r="D35" s="7"/>
-      <c r="E35" s="3"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="10"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36">
+      <c r="A36" s="5">
         <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" s="5">
         <v>1</v>
       </c>
-      <c r="D36" s="7"/>
-      <c r="E36" s="3"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="10"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37">
+      <c r="A37" s="5">
         <v>35</v>
       </c>
       <c r="B37" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C37" s="5">
         <v>8</v>
       </c>
-      <c r="D37" s="7"/>
-      <c r="E37" s="3"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="10"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38">
+      <c r="A38" s="5">
         <v>36</v>
       </c>
       <c r="B38" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="6">
+      <c r="C38" s="5">
         <v>2</v>
       </c>
-      <c r="D38" s="7"/>
-      <c r="E38" s="3"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="10"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39">
+      <c r="A39" s="5">
         <v>37</v>
       </c>
       <c r="B39" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="6">
+      <c r="C39" s="5">
         <v>9</v>
       </c>
-      <c r="D39" s="7"/>
-      <c r="E39" s="3"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="10"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40">
+      <c r="A40" s="5">
         <v>38</v>
       </c>
       <c r="B40" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="6">
+      <c r="C40" s="5">
         <v>18</v>
       </c>
-      <c r="D40" s="7"/>
-      <c r="E40" s="3"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="10"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41">
+      <c r="A41" s="5">
         <v>39</v>
       </c>
       <c r="B41" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="6">
+      <c r="C41" s="5">
         <v>14</v>
       </c>
-      <c r="D41" s="7"/>
-      <c r="E41" s="3"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="10"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42">
+      <c r="A42" s="5">
         <v>40</v>
       </c>
       <c r="B42" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="6">
+      <c r="C42" s="5">
         <v>27</v>
       </c>
-      <c r="D42" s="7"/>
-      <c r="E42" s="3"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="10"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43">
+      <c r="A43" s="5">
         <v>41</v>
       </c>
       <c r="B43" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="6">
+      <c r="C43" s="5">
         <v>45</v>
       </c>
-      <c r="D43" s="7"/>
-      <c r="E43" s="3"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="10"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44">
+      <c r="A44" s="5">
         <v>42</v>
       </c>
       <c r="B44" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="6">
+      <c r="C44" s="5">
         <v>7</v>
       </c>
-      <c r="D44" s="7"/>
-      <c r="E44" s="3"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="10"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45">
+      <c r="A45" s="5">
         <v>43</v>
       </c>
       <c r="B45" t="s">
         <v>44</v>
       </c>
-      <c r="C45" s="6">
+      <c r="C45" s="5">
         <v>1</v>
       </c>
-      <c r="D45" s="7"/>
-      <c r="E45" s="3"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="10"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46">
+      <c r="A46" s="5">
         <v>44</v>
       </c>
       <c r="B46" t="s">
         <v>45</v>
       </c>
-      <c r="C46" s="6">
+      <c r="C46" s="5">
         <v>15</v>
       </c>
-      <c r="D46" s="7"/>
-      <c r="E46" s="3"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="10"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47">
+      <c r="A47" s="5">
         <v>45</v>
       </c>
       <c r="B47" t="s">
         <v>46</v>
       </c>
-      <c r="C47" s="6">
+      <c r="C47" s="5">
         <v>12</v>
       </c>
-      <c r="D47" s="7"/>
-      <c r="E47" s="3"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="10"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48">
+      <c r="A48" s="5">
         <v>46</v>
       </c>
       <c r="B48" t="s">
         <v>47</v>
       </c>
-      <c r="C48" s="6">
+      <c r="C48" s="5">
         <v>1</v>
       </c>
-      <c r="D48" s="7"/>
-      <c r="E48" s="3"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="10"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49">
+      <c r="A49" s="5">
         <v>47</v>
       </c>
       <c r="B49" t="s">
         <v>48</v>
       </c>
-      <c r="C49" s="6">
+      <c r="C49" s="5">
         <v>24</v>
       </c>
-      <c r="D49" s="7"/>
-      <c r="E49" s="3"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="10"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50">
+      <c r="A50" s="5">
         <v>48</v>
       </c>
       <c r="B50" t="s">
         <v>49</v>
       </c>
-      <c r="C50" s="6">
+      <c r="C50" s="5">
         <v>2</v>
       </c>
-      <c r="D50" s="7"/>
-      <c r="E50" s="3"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="10"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51">
+      <c r="A51" s="5">
         <v>49</v>
       </c>
       <c r="B51" t="s">
         <v>50</v>
       </c>
-      <c r="C51" s="6">
+      <c r="C51" s="5">
         <v>6</v>
       </c>
-      <c r="D51" s="7"/>
-      <c r="E51" s="3"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="10"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52">
+      <c r="A52" s="5">
         <v>50</v>
       </c>
       <c r="B52" t="s">
         <v>51</v>
       </c>
-      <c r="C52" s="6">
+      <c r="C52" s="5">
         <v>2</v>
       </c>
-      <c r="D52" s="7"/>
-      <c r="E52" s="3"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="10"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53">
+      <c r="A53" s="5">
         <v>51</v>
       </c>
       <c r="B53" t="s">
         <v>52</v>
       </c>
-      <c r="C53" s="6">
+      <c r="C53" s="5">
         <v>22</v>
       </c>
-      <c r="D53" s="7"/>
-      <c r="E53" s="3"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="10"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54">
+      <c r="A54" s="5">
         <v>52</v>
       </c>
       <c r="B54" t="s">
         <v>53</v>
       </c>
-      <c r="C54" s="6">
+      <c r="C54" s="5">
         <v>8</v>
       </c>
-      <c r="D54" s="7"/>
-      <c r="E54" s="3"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="10"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55">
+      <c r="A55" s="5">
         <v>53</v>
       </c>
       <c r="B55" t="s">
         <v>54</v>
       </c>
-      <c r="C55" s="6">
+      <c r="C55" s="5">
         <v>1</v>
       </c>
-      <c r="D55" s="7"/>
-      <c r="E55" s="3"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="10"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56">
+      <c r="A56" s="5">
         <v>54</v>
       </c>
       <c r="B56" t="s">
         <v>55</v>
       </c>
-      <c r="C56" s="6">
+      <c r="C56" s="5">
         <v>3</v>
       </c>
-      <c r="D56" s="7"/>
-      <c r="E56" s="3"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="10"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57">
+      <c r="A57" s="5">
         <v>55</v>
       </c>
       <c r="B57" t="s">
         <v>56</v>
       </c>
-      <c r="C57" s="6">
+      <c r="C57" s="5">
         <v>7</v>
       </c>
-      <c r="D57" s="7"/>
-      <c r="E57" s="3"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="10"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58">
+      <c r="A58" s="5">
         <v>56</v>
       </c>
       <c r="B58" t="s">
         <v>57</v>
       </c>
-      <c r="C58" s="6">
+      <c r="C58" s="5">
         <v>3</v>
       </c>
-      <c r="D58" s="7"/>
-      <c r="E58" s="3"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="10"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59">
+      <c r="A59" s="5">
         <v>57</v>
       </c>
       <c r="B59" t="s">
         <v>58</v>
       </c>
-      <c r="C59" s="6">
+      <c r="C59" s="5">
         <v>4</v>
       </c>
-      <c r="D59" s="7"/>
-      <c r="E59" s="3"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="10"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60">
+      <c r="A60" s="5">
         <v>58</v>
       </c>
       <c r="B60" t="s">
         <v>59</v>
       </c>
-      <c r="C60" s="6">
+      <c r="C60" s="5">
         <v>6</v>
       </c>
-      <c r="D60" s="7"/>
-      <c r="E60" s="3"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="10"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61">
+      <c r="A61" s="5">
         <v>59</v>
       </c>
       <c r="B61" t="s">
         <v>60</v>
       </c>
-      <c r="C61" s="6">
+      <c r="C61" s="5">
         <v>2</v>
       </c>
-      <c r="D61" s="7"/>
-      <c r="E61" s="3"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="10"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62">
+      <c r="A62" s="5">
         <v>60</v>
       </c>
       <c r="B62" t="s">
         <v>61</v>
       </c>
-      <c r="C62" s="6">
+      <c r="C62" s="5">
         <v>2</v>
       </c>
-      <c r="D62" s="7"/>
-      <c r="E62" s="3"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="10"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63">
+      <c r="A63" s="5">
         <v>61</v>
       </c>
       <c r="B63" t="s">
         <v>62</v>
       </c>
-      <c r="C63" s="6">
+      <c r="C63" s="5">
         <v>1</v>
       </c>
-      <c r="D63" s="7"/>
-      <c r="E63" s="3"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="10"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64">
+      <c r="A64" s="5">
         <v>62</v>
       </c>
       <c r="B64" t="s">
         <v>63</v>
       </c>
-      <c r="C64" s="6">
+      <c r="C64" s="5">
         <v>11</v>
       </c>
-      <c r="D64" s="7"/>
-      <c r="E64" s="3"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="10"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65">
+      <c r="A65" s="5">
         <v>63</v>
       </c>
       <c r="B65" t="s">
         <v>64</v>
       </c>
-      <c r="C65" s="6">
+      <c r="C65" s="5">
         <v>4</v>
       </c>
-      <c r="D65" s="7"/>
-      <c r="E65" s="3"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="10"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66">
+      <c r="A66" s="5">
         <v>64</v>
       </c>
       <c r="B66" t="s">
         <v>65</v>
       </c>
-      <c r="C66" s="6">
+      <c r="C66" s="5">
         <v>6</v>
       </c>
-      <c r="D66" s="7"/>
-      <c r="E66" s="2"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="9">
+        <v>6</v>
+      </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67">
+      <c r="A67" s="5">
         <v>65</v>
       </c>
       <c r="B67" t="s">
         <v>66</v>
       </c>
-      <c r="C67" s="6">
+      <c r="C67" s="5">
         <v>38</v>
       </c>
-      <c r="D67" s="7"/>
-      <c r="E67" s="3"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="10"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68">
+      <c r="A68" s="5">
         <v>66</v>
       </c>
       <c r="B68" t="s">
         <v>67</v>
       </c>
-      <c r="C68" s="6">
+      <c r="C68" s="5">
         <v>4</v>
       </c>
-      <c r="D68" s="7"/>
-      <c r="E68" s="3"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="10"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69">
+      <c r="A69" s="5">
         <v>67</v>
       </c>
       <c r="B69" t="s">
         <v>68</v>
       </c>
-      <c r="C69" s="6">
+      <c r="C69" s="5">
         <v>25</v>
       </c>
-      <c r="D69" s="7"/>
-      <c r="E69" s="3"/>
+      <c r="D69" s="11"/>
+      <c r="E69" s="10"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70">
+      <c r="A70" s="5">
         <v>68</v>
       </c>
       <c r="B70" t="s">
         <v>69</v>
       </c>
-      <c r="C70" s="6">
+      <c r="C70" s="5">
         <v>19</v>
       </c>
-      <c r="D70" s="7"/>
-      <c r="E70" s="3"/>
+      <c r="D70" s="11"/>
+      <c r="E70" s="10"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>77</v>
+      </c>
+      <c r="C72" s="5">
+        <f>SUM(C2:C70)</f>
+        <v>872</v>
+      </c>
+      <c r="D72" s="8">
+        <v>1</v>
+      </c>
+      <c r="E72" s="7">
+        <f>(SUM(E2:E70)/SUM(C2:C70))</f>
+        <v>0.17201834862385321</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Scraper2 tasks complete, merge with main branch upcoming
</commit_message>
<xml_diff>
--- a/Docs/HistoryScrapeStatus.xlsx
+++ b/Docs/HistoryScrapeStatus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpete\Documents\Projects\CarStats\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3AE5B4-3F13-4930-A281-0E712B051C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F250FFF1-BF80-4A61-A503-B3F68DE40D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-3435" windowWidth="29040" windowHeight="15840" xr2:uid="{84160147-604C-44EB-89D6-C5A3DE91A955}"/>
+    <workbookView xWindow="-28920" yWindow="-3435" windowWidth="29040" windowHeight="15840" xr2:uid="{84160147-604C-44EB-89D6-C5A3DE91A955}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>Index</t>
   </si>
@@ -273,15 +273,15 @@
   </si>
   <si>
     <t>Size (base links)</t>
+  </si>
+  <si>
+    <t>% of total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000%"/>
-  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -373,7 +373,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -384,9 +384,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -399,6 +396,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -717,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2B1DA9D-AC09-4F91-8BA6-4CCF32CADB06}">
-  <dimension ref="A1:L72"/>
+  <dimension ref="A1:M72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -728,41 +733,45 @@
     <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1"/>
-    <col min="5" max="5" width="19.77734375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
+    <col min="6" max="6" width="19.77734375" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:13" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12" t="s">
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>0</v>
       </c>
@@ -772,16 +781,20 @@
       <c r="C2" s="5">
         <v>11</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="9">
+      <c r="D2" s="10">
+        <f>(C2/C72)</f>
+        <v>1.261467889908257E-2</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="6">
         <v>11</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" t="s">
+      <c r="L2" s="2"/>
+      <c r="M2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -791,16 +804,20 @@
       <c r="C3" s="5">
         <v>1</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="9">
+      <c r="D3" s="10">
+        <f>(C3/C72)</f>
+        <v>1.1467889908256881E-3</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="6">
         <v>1</v>
       </c>
-      <c r="K3" s="1"/>
-      <c r="L3" t="s">
+      <c r="L3" s="1"/>
+      <c r="M3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -810,16 +827,20 @@
       <c r="C4" s="5">
         <v>9</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="9">
+      <c r="D4" s="10">
+        <f>(C4/C72)</f>
+        <v>1.0321100917431193E-2</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="6">
         <v>9</v>
       </c>
-      <c r="K4" s="3"/>
-      <c r="L4" t="s">
+      <c r="L4" s="3"/>
+      <c r="M4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -829,12 +850,16 @@
       <c r="C5" s="5">
         <v>12</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="9">
+      <c r="D5" s="10">
+        <f>(C5/C72)</f>
+        <v>1.3761467889908258E-2</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="6">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -844,12 +869,16 @@
       <c r="C6" s="5">
         <v>40</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="9">
+      <c r="D6" s="10">
+        <f>(C6/C72)</f>
+        <v>4.5871559633027525E-2</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="6">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -859,12 +888,16 @@
       <c r="C7" s="5">
         <v>9</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="9">
+      <c r="D7" s="10">
+        <f>(C7/C72)</f>
+        <v>1.0321100917431193E-2</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="6">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -874,12 +907,16 @@
       <c r="C8" s="5">
         <v>43</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="9">
+      <c r="D8" s="10">
+        <f>(C8/C72)</f>
+        <v>4.931192660550459E-2</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="6">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -889,12 +926,16 @@
       <c r="C9" s="5">
         <v>2</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="9">
+      <c r="D9" s="10">
+        <f>(C9/C72)</f>
+        <v>2.2935779816513763E-3</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -904,12 +945,16 @@
       <c r="C10" s="5">
         <v>3</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="9">
+      <c r="D10" s="10">
+        <f>(C10/C72)</f>
+        <v>3.4403669724770644E-3</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -919,12 +964,16 @@
       <c r="C11" s="5">
         <v>13</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="9">
+      <c r="D11" s="10">
+        <f>(C11/C72)</f>
+        <v>1.4908256880733946E-2</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="6">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -934,12 +983,16 @@
       <c r="C12" s="5">
         <v>1</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="9">
+      <c r="D12" s="10">
+        <f>(C12/C72)</f>
+        <v>1.1467889908256881E-3</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -949,10 +1002,16 @@
       <c r="C13" s="5">
         <v>23</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D13" s="10">
+        <f>(C13/C72)</f>
+        <v>2.6376146788990827E-2</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -962,10 +1021,16 @@
       <c r="C14" s="5">
         <v>40</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="10"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D14" s="10">
+        <f>(C14/C72)</f>
+        <v>4.5871559633027525E-2</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -975,10 +1040,16 @@
       <c r="C15" s="5">
         <v>10</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="10"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D15" s="10">
+        <f>C15/C72</f>
+        <v>1.1467889908256881E-2</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -988,10 +1059,16 @@
       <c r="C16" s="5">
         <v>17</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="10"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D16" s="10">
+        <f>C16/C72</f>
+        <v>1.9495412844036698E-2</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>15</v>
       </c>
@@ -1001,10 +1078,16 @@
       <c r="C17" s="5">
         <v>16</v>
       </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="10"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D17" s="10">
+        <f>C17/C72</f>
+        <v>1.834862385321101E-2</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -1014,10 +1097,16 @@
       <c r="C18" s="5">
         <v>6</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D18" s="10">
+        <f>C18/C72</f>
+        <v>6.8807339449541288E-3</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>17</v>
       </c>
@@ -1027,10 +1116,16 @@
       <c r="C19" s="5">
         <v>5</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="10"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D19" s="10">
+        <f>C19/C72</f>
+        <v>5.7339449541284407E-3</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -1040,10 +1135,16 @@
       <c r="C20" s="5">
         <v>39</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="10"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D20" s="10">
+        <f>C20/C72</f>
+        <v>4.4724770642201837E-2</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="6">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>19</v>
       </c>
@@ -1053,10 +1154,16 @@
       <c r="C21" s="5">
         <v>11</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="10"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D21" s="10">
+        <f>C21/C72</f>
+        <v>1.261467889908257E-2</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -1066,10 +1173,14 @@
       <c r="C22" s="5">
         <v>11</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="10"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D22" s="10">
+        <f>C22/C72</f>
+        <v>1.261467889908257E-2</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>21</v>
       </c>
@@ -1079,10 +1190,14 @@
       <c r="C23" s="5">
         <v>19</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="10"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D23" s="10">
+        <f>C23/C72</f>
+        <v>2.1788990825688075E-2</v>
+      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>22</v>
       </c>
@@ -1092,10 +1207,14 @@
       <c r="C24" s="5">
         <v>2</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="10"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D24" s="10">
+        <f>C24/C72</f>
+        <v>2.2935779816513763E-3</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>23</v>
       </c>
@@ -1105,10 +1224,14 @@
       <c r="C25" s="5">
         <v>36</v>
       </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="10"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D25" s="10">
+        <f>C25/C72</f>
+        <v>4.1284403669724773E-2</v>
+      </c>
+      <c r="E25" s="8"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>24</v>
       </c>
@@ -1118,10 +1241,14 @@
       <c r="C26" s="5">
         <v>16</v>
       </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="10"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D26" s="10">
+        <f>C26/C72</f>
+        <v>1.834862385321101E-2</v>
+      </c>
+      <c r="E26" s="8"/>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>25</v>
       </c>
@@ -1131,10 +1258,14 @@
       <c r="C27" s="5">
         <v>14</v>
       </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="10"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D27" s="10">
+        <f>C27/C72</f>
+        <v>1.6055045871559634E-2</v>
+      </c>
+      <c r="E27" s="8"/>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>26</v>
       </c>
@@ -1144,10 +1275,14 @@
       <c r="C28" s="5">
         <v>16</v>
       </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="10"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D28" s="10">
+        <f>C28/C72</f>
+        <v>1.834862385321101E-2</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>27</v>
       </c>
@@ -1157,10 +1292,14 @@
       <c r="C29" s="5">
         <v>1</v>
       </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="10"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D29" s="10">
+        <f>C29/C72</f>
+        <v>1.1467889908256881E-3</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>28</v>
       </c>
@@ -1170,10 +1309,14 @@
       <c r="C30" s="5">
         <v>27</v>
       </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="10"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D30" s="10">
+        <f>C30/C72</f>
+        <v>3.096330275229358E-2</v>
+      </c>
+      <c r="E30" s="8"/>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>29</v>
       </c>
@@ -1183,10 +1326,14 @@
       <c r="C31" s="5">
         <v>2</v>
       </c>
-      <c r="D31" s="11"/>
-      <c r="E31" s="10"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D31" s="10">
+        <f>C31/C72</f>
+        <v>2.2935779816513763E-3</v>
+      </c>
+      <c r="E31" s="8"/>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>30</v>
       </c>
@@ -1196,10 +1343,14 @@
       <c r="C32" s="5">
         <v>9</v>
       </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="10"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D32" s="10">
+        <f>C32/C72</f>
+        <v>1.0321100917431193E-2</v>
+      </c>
+      <c r="E32" s="8"/>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>31</v>
       </c>
@@ -1209,10 +1360,14 @@
       <c r="C33" s="5">
         <v>14</v>
       </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="10"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D33" s="10">
+        <f>C33/C72</f>
+        <v>1.6055045871559634E-2</v>
+      </c>
+      <c r="E33" s="8"/>
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>32</v>
       </c>
@@ -1222,10 +1377,14 @@
       <c r="C34" s="5">
         <v>22</v>
       </c>
-      <c r="D34" s="11"/>
-      <c r="E34" s="10"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D34" s="10">
+        <f>C34/C72</f>
+        <v>2.5229357798165139E-2</v>
+      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>33</v>
       </c>
@@ -1235,10 +1394,14 @@
       <c r="C35" s="5">
         <v>12</v>
       </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="10"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D35" s="10">
+        <f>C35/C72</f>
+        <v>1.3761467889908258E-2</v>
+      </c>
+      <c r="E35" s="8"/>
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>34</v>
       </c>
@@ -1248,10 +1411,14 @@
       <c r="C36" s="5">
         <v>1</v>
       </c>
-      <c r="D36" s="11"/>
-      <c r="E36" s="10"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D36" s="10">
+        <f>C36/C72</f>
+        <v>1.1467889908256881E-3</v>
+      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>35</v>
       </c>
@@ -1261,10 +1428,14 @@
       <c r="C37" s="5">
         <v>8</v>
       </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="10"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D37" s="10">
+        <f>C37/C72</f>
+        <v>9.1743119266055051E-3</v>
+      </c>
+      <c r="E37" s="8"/>
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>36</v>
       </c>
@@ -1274,10 +1445,14 @@
       <c r="C38" s="5">
         <v>2</v>
       </c>
-      <c r="D38" s="11"/>
-      <c r="E38" s="10"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D38" s="10">
+        <f>C38/C72</f>
+        <v>2.2935779816513763E-3</v>
+      </c>
+      <c r="E38" s="8"/>
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>37</v>
       </c>
@@ -1287,10 +1462,14 @@
       <c r="C39" s="5">
         <v>9</v>
       </c>
-      <c r="D39" s="11"/>
-      <c r="E39" s="10"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D39" s="10">
+        <f>C39/C72</f>
+        <v>1.0321100917431193E-2</v>
+      </c>
+      <c r="E39" s="8"/>
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>38</v>
       </c>
@@ -1300,10 +1479,14 @@
       <c r="C40" s="5">
         <v>18</v>
       </c>
-      <c r="D40" s="11"/>
-      <c r="E40" s="10"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D40" s="10">
+        <f>C40/C72</f>
+        <v>2.0642201834862386E-2</v>
+      </c>
+      <c r="E40" s="8"/>
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>39</v>
       </c>
@@ -1313,10 +1496,14 @@
       <c r="C41" s="5">
         <v>14</v>
       </c>
-      <c r="D41" s="11"/>
-      <c r="E41" s="10"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D41" s="10">
+        <f>C41/C72</f>
+        <v>1.6055045871559634E-2</v>
+      </c>
+      <c r="E41" s="8"/>
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>40</v>
       </c>
@@ -1326,10 +1513,14 @@
       <c r="C42" s="5">
         <v>27</v>
       </c>
-      <c r="D42" s="11"/>
-      <c r="E42" s="10"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D42" s="10">
+        <f>C42/C72</f>
+        <v>3.096330275229358E-2</v>
+      </c>
+      <c r="E42" s="8"/>
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>41</v>
       </c>
@@ -1339,10 +1530,14 @@
       <c r="C43" s="5">
         <v>45</v>
       </c>
-      <c r="D43" s="11"/>
-      <c r="E43" s="10"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D43" s="10">
+        <f>C43/C72</f>
+        <v>5.1605504587155966E-2</v>
+      </c>
+      <c r="E43" s="8"/>
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>42</v>
       </c>
@@ -1352,10 +1547,14 @@
       <c r="C44" s="5">
         <v>7</v>
       </c>
-      <c r="D44" s="11"/>
-      <c r="E44" s="10"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D44" s="10">
+        <f>C44/C72</f>
+        <v>8.027522935779817E-3</v>
+      </c>
+      <c r="E44" s="8"/>
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>43</v>
       </c>
@@ -1365,10 +1564,14 @@
       <c r="C45" s="5">
         <v>1</v>
       </c>
-      <c r="D45" s="11"/>
-      <c r="E45" s="10"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D45" s="10">
+        <f>C45/C72</f>
+        <v>1.1467889908256881E-3</v>
+      </c>
+      <c r="E45" s="8"/>
+      <c r="F45" s="7"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>44</v>
       </c>
@@ -1378,10 +1581,14 @@
       <c r="C46" s="5">
         <v>15</v>
       </c>
-      <c r="D46" s="11"/>
-      <c r="E46" s="10"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D46" s="10">
+        <f>C46/C72</f>
+        <v>1.7201834862385322E-2</v>
+      </c>
+      <c r="E46" s="8"/>
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>45</v>
       </c>
@@ -1391,10 +1598,14 @@
       <c r="C47" s="5">
         <v>12</v>
       </c>
-      <c r="D47" s="11"/>
-      <c r="E47" s="10"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D47" s="10">
+        <f>C47/C72</f>
+        <v>1.3761467889908258E-2</v>
+      </c>
+      <c r="E47" s="8"/>
+      <c r="F47" s="7"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>46</v>
       </c>
@@ -1404,10 +1615,14 @@
       <c r="C48" s="5">
         <v>1</v>
       </c>
-      <c r="D48" s="11"/>
-      <c r="E48" s="10"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D48" s="10">
+        <f>C48/C72</f>
+        <v>1.1467889908256881E-3</v>
+      </c>
+      <c r="E48" s="8"/>
+      <c r="F48" s="7"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>47</v>
       </c>
@@ -1417,10 +1632,14 @@
       <c r="C49" s="5">
         <v>24</v>
       </c>
-      <c r="D49" s="11"/>
-      <c r="E49" s="10"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D49" s="10">
+        <f>C49/C72</f>
+        <v>2.7522935779816515E-2</v>
+      </c>
+      <c r="E49" s="8"/>
+      <c r="F49" s="7"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>48</v>
       </c>
@@ -1430,10 +1649,14 @@
       <c r="C50" s="5">
         <v>2</v>
       </c>
-      <c r="D50" s="11"/>
-      <c r="E50" s="10"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D50" s="10">
+        <f>C50/C72</f>
+        <v>2.2935779816513763E-3</v>
+      </c>
+      <c r="E50" s="8"/>
+      <c r="F50" s="7"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>49</v>
       </c>
@@ -1443,10 +1666,14 @@
       <c r="C51" s="5">
         <v>6</v>
       </c>
-      <c r="D51" s="11"/>
-      <c r="E51" s="10"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D51" s="10">
+        <f>C51/C72</f>
+        <v>6.8807339449541288E-3</v>
+      </c>
+      <c r="E51" s="8"/>
+      <c r="F51" s="7"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>50</v>
       </c>
@@ -1456,10 +1683,14 @@
       <c r="C52" s="5">
         <v>2</v>
       </c>
-      <c r="D52" s="11"/>
-      <c r="E52" s="10"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D52" s="10">
+        <f>C52/C72</f>
+        <v>2.2935779816513763E-3</v>
+      </c>
+      <c r="E52" s="8"/>
+      <c r="F52" s="7"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>51</v>
       </c>
@@ -1469,10 +1700,14 @@
       <c r="C53" s="5">
         <v>22</v>
       </c>
-      <c r="D53" s="11"/>
-      <c r="E53" s="10"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D53" s="10">
+        <f>C53/C72</f>
+        <v>2.5229357798165139E-2</v>
+      </c>
+      <c r="E53" s="8"/>
+      <c r="F53" s="7"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>52</v>
       </c>
@@ -1482,10 +1717,14 @@
       <c r="C54" s="5">
         <v>8</v>
       </c>
-      <c r="D54" s="11"/>
-      <c r="E54" s="10"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D54" s="10">
+        <f>C54/C72</f>
+        <v>9.1743119266055051E-3</v>
+      </c>
+      <c r="E54" s="8"/>
+      <c r="F54" s="7"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <v>53</v>
       </c>
@@ -1495,10 +1734,14 @@
       <c r="C55" s="5">
         <v>1</v>
       </c>
-      <c r="D55" s="11"/>
-      <c r="E55" s="10"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D55" s="10">
+        <f>C55/C72</f>
+        <v>1.1467889908256881E-3</v>
+      </c>
+      <c r="E55" s="8"/>
+      <c r="F55" s="7"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
         <v>54</v>
       </c>
@@ -1508,10 +1751,14 @@
       <c r="C56" s="5">
         <v>3</v>
       </c>
-      <c r="D56" s="11"/>
-      <c r="E56" s="10"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D56" s="10">
+        <f>C56/C72</f>
+        <v>3.4403669724770644E-3</v>
+      </c>
+      <c r="E56" s="8"/>
+      <c r="F56" s="7"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
         <v>55</v>
       </c>
@@ -1521,10 +1768,14 @@
       <c r="C57" s="5">
         <v>7</v>
       </c>
-      <c r="D57" s="11"/>
-      <c r="E57" s="10"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D57" s="10">
+        <f>C57/C72</f>
+        <v>8.027522935779817E-3</v>
+      </c>
+      <c r="E57" s="8"/>
+      <c r="F57" s="7"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
         <v>56</v>
       </c>
@@ -1534,10 +1785,14 @@
       <c r="C58" s="5">
         <v>3</v>
       </c>
-      <c r="D58" s="11"/>
-      <c r="E58" s="10"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D58" s="10">
+        <f>C58/C72</f>
+        <v>3.4403669724770644E-3</v>
+      </c>
+      <c r="E58" s="8"/>
+      <c r="F58" s="7"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="5">
         <v>57</v>
       </c>
@@ -1547,10 +1802,14 @@
       <c r="C59" s="5">
         <v>4</v>
       </c>
-      <c r="D59" s="11"/>
-      <c r="E59" s="10"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D59" s="10">
+        <f>C59/C72</f>
+        <v>4.5871559633027525E-3</v>
+      </c>
+      <c r="E59" s="8"/>
+      <c r="F59" s="7"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
         <v>58</v>
       </c>
@@ -1560,10 +1819,14 @@
       <c r="C60" s="5">
         <v>6</v>
       </c>
-      <c r="D60" s="11"/>
-      <c r="E60" s="10"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D60" s="10">
+        <f>C60/C72</f>
+        <v>6.8807339449541288E-3</v>
+      </c>
+      <c r="E60" s="8"/>
+      <c r="F60" s="7"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="5">
         <v>59</v>
       </c>
@@ -1573,10 +1836,14 @@
       <c r="C61" s="5">
         <v>2</v>
       </c>
-      <c r="D61" s="11"/>
-      <c r="E61" s="10"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D61" s="10">
+        <f>C61/C72</f>
+        <v>2.2935779816513763E-3</v>
+      </c>
+      <c r="E61" s="8"/>
+      <c r="F61" s="7"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="5">
         <v>60</v>
       </c>
@@ -1586,10 +1853,14 @@
       <c r="C62" s="5">
         <v>2</v>
       </c>
-      <c r="D62" s="11"/>
-      <c r="E62" s="10"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D62" s="10">
+        <f>C62/C72</f>
+        <v>2.2935779816513763E-3</v>
+      </c>
+      <c r="E62" s="8"/>
+      <c r="F62" s="7"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="5">
         <v>61</v>
       </c>
@@ -1599,10 +1870,14 @@
       <c r="C63" s="5">
         <v>1</v>
       </c>
-      <c r="D63" s="11"/>
-      <c r="E63" s="10"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D63" s="10">
+        <f>C63/C72</f>
+        <v>1.1467889908256881E-3</v>
+      </c>
+      <c r="E63" s="8"/>
+      <c r="F63" s="7"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="5">
         <v>62</v>
       </c>
@@ -1612,10 +1887,14 @@
       <c r="C64" s="5">
         <v>11</v>
       </c>
-      <c r="D64" s="11"/>
-      <c r="E64" s="10"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D64" s="10">
+        <f>C64/C72</f>
+        <v>1.261467889908257E-2</v>
+      </c>
+      <c r="E64" s="8"/>
+      <c r="F64" s="7"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="5">
         <v>63</v>
       </c>
@@ -1625,10 +1904,14 @@
       <c r="C65" s="5">
         <v>4</v>
       </c>
-      <c r="D65" s="11"/>
-      <c r="E65" s="10"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D65" s="10">
+        <f>C65/C72</f>
+        <v>4.5871559633027525E-3</v>
+      </c>
+      <c r="E65" s="8"/>
+      <c r="F65" s="7"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="5">
         <v>64</v>
       </c>
@@ -1638,12 +1921,16 @@
       <c r="C66" s="5">
         <v>6</v>
       </c>
-      <c r="D66" s="11"/>
-      <c r="E66" s="9">
+      <c r="D66" s="10">
+        <f>C66/C72</f>
+        <v>6.8807339449541288E-3</v>
+      </c>
+      <c r="E66" s="8"/>
+      <c r="F66" s="6">
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="5">
         <v>65</v>
       </c>
@@ -1653,10 +1940,14 @@
       <c r="C67" s="5">
         <v>38</v>
       </c>
-      <c r="D67" s="11"/>
-      <c r="E67" s="10"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D67" s="10">
+        <f>C67/C72</f>
+        <v>4.3577981651376149E-2</v>
+      </c>
+      <c r="E67" s="8"/>
+      <c r="F67" s="7"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="5">
         <v>66</v>
       </c>
@@ -1666,10 +1957,14 @@
       <c r="C68" s="5">
         <v>4</v>
       </c>
-      <c r="D68" s="11"/>
-      <c r="E68" s="10"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D68" s="10">
+        <f>C68/C72</f>
+        <v>4.5871559633027525E-3</v>
+      </c>
+      <c r="E68" s="8"/>
+      <c r="F68" s="7"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="5">
         <v>67</v>
       </c>
@@ -1679,10 +1974,14 @@
       <c r="C69" s="5">
         <v>25</v>
       </c>
-      <c r="D69" s="11"/>
-      <c r="E69" s="10"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D69" s="10">
+        <f>C69/C72</f>
+        <v>2.8669724770642203E-2</v>
+      </c>
+      <c r="E69" s="8"/>
+      <c r="F69" s="7"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="5">
         <v>68</v>
       </c>
@@ -1692,10 +1991,14 @@
       <c r="C70" s="5">
         <v>19</v>
       </c>
-      <c r="D70" s="11"/>
-      <c r="E70" s="10"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D70" s="10">
+        <f>C70/C72</f>
+        <v>2.1788990825688075E-2</v>
+      </c>
+      <c r="E70" s="8"/>
+      <c r="F70" s="7"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>77</v>
       </c>
@@ -1703,12 +2006,16 @@
         <f>SUM(C2:C70)</f>
         <v>872</v>
       </c>
-      <c r="D72" s="8">
+      <c r="D72" s="10">
+        <f>C72/C72</f>
         <v>1</v>
       </c>
-      <c r="E72" s="7">
-        <f>(SUM(E2:E70)/SUM(C2:C70))</f>
-        <v>0.17201834862385321</v>
+      <c r="E72" s="12">
+        <v>1</v>
+      </c>
+      <c r="F72" s="13">
+        <f>(SUM(F2:F70)/SUM(C2:C70))</f>
+        <v>0.36353211009174313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Speed up in scraoer, continued obtaining data
</commit_message>
<xml_diff>
--- a/Docs/HistoryScrapeStatus.xlsx
+++ b/Docs/HistoryScrapeStatus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpete\Documents\Projects\CarStats\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F250FFF1-BF80-4A61-A503-B3F68DE40D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D777229B-DF12-4E40-B861-756F985BEF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3435" windowWidth="29040" windowHeight="15840" xr2:uid="{84160147-604C-44EB-89D6-C5A3DE91A955}"/>
+    <workbookView xWindow="-57720" yWindow="-3435" windowWidth="29040" windowHeight="15840" xr2:uid="{84160147-604C-44EB-89D6-C5A3DE91A955}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -373,7 +373,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -403,7 +403,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -725,7 +724,7 @@
   <dimension ref="A1:M72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -735,7 +734,7 @@
     <col min="3" max="3" width="17.33203125" style="5" customWidth="1"/>
     <col min="4" max="4" width="11.21875" style="10" customWidth="1"/>
     <col min="5" max="5" width="14.88671875" customWidth="1"/>
-    <col min="6" max="6" width="19.77734375" customWidth="1"/>
+    <col min="6" max="6" width="19.77734375" style="5" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4.21875" bestFit="1" customWidth="1"/>
@@ -1178,7 +1177,9 @@
         <v>1.261467889908257E-2</v>
       </c>
       <c r="E22" s="8"/>
-      <c r="F22" s="7"/>
+      <c r="F22" s="6">
+        <v>11</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
@@ -1195,7 +1196,9 @@
         <v>2.1788990825688075E-2</v>
       </c>
       <c r="E23" s="8"/>
-      <c r="F23" s="7"/>
+      <c r="F23" s="6">
+        <v>19</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
@@ -1212,7 +1215,9 @@
         <v>2.2935779816513763E-3</v>
       </c>
       <c r="E24" s="8"/>
-      <c r="F24" s="7"/>
+      <c r="F24" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
@@ -1229,7 +1234,9 @@
         <v>4.1284403669724773E-2</v>
       </c>
       <c r="E25" s="8"/>
-      <c r="F25" s="7"/>
+      <c r="F25" s="6">
+        <v>36</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
@@ -1246,7 +1253,9 @@
         <v>1.834862385321101E-2</v>
       </c>
       <c r="E26" s="8"/>
-      <c r="F26" s="7"/>
+      <c r="F26" s="6">
+        <v>16</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
@@ -2013,9 +2022,9 @@
       <c r="E72" s="12">
         <v>1</v>
       </c>
-      <c r="F72" s="13">
+      <c r="F72" s="10">
         <f>(SUM(F2:F70)/SUM(C2:C70))</f>
-        <v>0.36353211009174313</v>
+        <v>0.45986238532110091</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enhancements to scraper, obtaining more data
</commit_message>
<xml_diff>
--- a/Docs/HistoryScrapeStatus.xlsx
+++ b/Docs/HistoryScrapeStatus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpete\Documents\Projects\CarStats\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D777229B-DF12-4E40-B861-756F985BEF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB51BE59-2F85-4E34-AD8C-AD790FD95F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-3435" windowWidth="29040" windowHeight="15840" xr2:uid="{84160147-604C-44EB-89D6-C5A3DE91A955}"/>
+    <workbookView xWindow="-28920" yWindow="-3435" windowWidth="29040" windowHeight="15840" xr2:uid="{84160147-604C-44EB-89D6-C5A3DE91A955}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -723,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2B1DA9D-AC09-4F91-8BA6-4CCF32CADB06}">
   <dimension ref="A1:M72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1272,7 +1272,9 @@
         <v>1.6055045871559634E-2</v>
       </c>
       <c r="E27" s="8"/>
-      <c r="F27" s="7"/>
+      <c r="F27" s="6">
+        <v>14</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
@@ -1289,7 +1291,9 @@
         <v>1.834862385321101E-2</v>
       </c>
       <c r="E28" s="8"/>
-      <c r="F28" s="7"/>
+      <c r="F28" s="6">
+        <v>16</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
@@ -1306,7 +1310,9 @@
         <v>1.1467889908256881E-3</v>
       </c>
       <c r="E29" s="8"/>
-      <c r="F29" s="7"/>
+      <c r="F29" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
@@ -1323,7 +1329,9 @@
         <v>3.096330275229358E-2</v>
       </c>
       <c r="E30" s="8"/>
-      <c r="F30" s="7"/>
+      <c r="F30" s="6">
+        <v>27</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
@@ -1340,7 +1348,9 @@
         <v>2.2935779816513763E-3</v>
       </c>
       <c r="E31" s="8"/>
-      <c r="F31" s="7"/>
+      <c r="F31" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
@@ -1357,7 +1367,9 @@
         <v>1.0321100917431193E-2</v>
       </c>
       <c r="E32" s="8"/>
-      <c r="F32" s="7"/>
+      <c r="F32" s="6">
+        <v>9</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
@@ -1374,7 +1386,9 @@
         <v>1.6055045871559634E-2</v>
       </c>
       <c r="E33" s="8"/>
-      <c r="F33" s="7"/>
+      <c r="F33" s="6">
+        <v>14</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
@@ -1391,7 +1405,9 @@
         <v>2.5229357798165139E-2</v>
       </c>
       <c r="E34" s="8"/>
-      <c r="F34" s="7"/>
+      <c r="F34" s="6">
+        <v>22</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
@@ -1408,7 +1424,9 @@
         <v>1.3761467889908258E-2</v>
       </c>
       <c r="E35" s="8"/>
-      <c r="F35" s="7"/>
+      <c r="F35" s="6">
+        <v>12</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
@@ -1425,7 +1443,9 @@
         <v>1.1467889908256881E-3</v>
       </c>
       <c r="E36" s="8"/>
-      <c r="F36" s="7"/>
+      <c r="F36" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
@@ -1442,7 +1462,9 @@
         <v>9.1743119266055051E-3</v>
       </c>
       <c r="E37" s="8"/>
-      <c r="F37" s="7"/>
+      <c r="F37" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
@@ -1459,7 +1481,9 @@
         <v>2.2935779816513763E-3</v>
       </c>
       <c r="E38" s="8"/>
-      <c r="F38" s="7"/>
+      <c r="F38" s="6">
+        <v>8</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
@@ -1476,7 +1500,9 @@
         <v>1.0321100917431193E-2</v>
       </c>
       <c r="E39" s="8"/>
-      <c r="F39" s="7"/>
+      <c r="F39" s="6">
+        <v>9</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
@@ -1493,7 +1519,9 @@
         <v>2.0642201834862386E-2</v>
       </c>
       <c r="E40" s="8"/>
-      <c r="F40" s="7"/>
+      <c r="F40" s="6">
+        <v>18</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
@@ -1510,7 +1538,9 @@
         <v>1.6055045871559634E-2</v>
       </c>
       <c r="E41" s="8"/>
-      <c r="F41" s="7"/>
+      <c r="F41" s="6">
+        <v>14</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
@@ -2024,7 +2054,7 @@
       </c>
       <c r="F72" s="10">
         <f>(SUM(F2:F70)/SUM(C2:C70))</f>
-        <v>0.45986238532110091</v>
+        <v>0.65252293577981646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clean up and finished data gathering, on to data processing
</commit_message>
<xml_diff>
--- a/Docs/HistoryScrapeStatus.xlsx
+++ b/Docs/HistoryScrapeStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpete\Documents\Projects\CarStats\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB51BE59-2F85-4E34-AD8C-AD790FD95F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8E3317-B1C0-4A4E-813E-2BBCA5D4F728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-3435" windowWidth="29040" windowHeight="15840" xr2:uid="{84160147-604C-44EB-89D6-C5A3DE91A955}"/>
   </bookViews>
@@ -373,7 +373,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -385,9 +385,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
@@ -402,7 +399,9 @@
     <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -723,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2B1DA9D-AC09-4F91-8BA6-4CCF32CADB06}">
   <dimension ref="A1:M72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -732,7 +731,7 @@
     <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" style="9" customWidth="1"/>
     <col min="5" max="5" width="14.88671875" customWidth="1"/>
     <col min="6" max="6" width="19.77734375" style="5" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
@@ -743,30 +742,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9" t="s">
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8" t="s">
         <v>70</v>
       </c>
     </row>
@@ -780,11 +779,11 @@
       <c r="C2" s="5">
         <v>11</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="9">
         <f>(C2/C72)</f>
         <v>1.261467889908257E-2</v>
       </c>
-      <c r="E2" s="8"/>
+      <c r="E2" s="7"/>
       <c r="F2" s="6">
         <v>11</v>
       </c>
@@ -803,11 +802,11 @@
       <c r="C3" s="5">
         <v>1</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <f>(C3/C72)</f>
         <v>1.1467889908256881E-3</v>
       </c>
-      <c r="E3" s="8"/>
+      <c r="E3" s="7"/>
       <c r="F3" s="6">
         <v>1</v>
       </c>
@@ -826,11 +825,11 @@
       <c r="C4" s="5">
         <v>9</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <f>(C4/C72)</f>
         <v>1.0321100917431193E-2</v>
       </c>
-      <c r="E4" s="8"/>
+      <c r="E4" s="7"/>
       <c r="F4" s="6">
         <v>9</v>
       </c>
@@ -849,11 +848,11 @@
       <c r="C5" s="5">
         <v>12</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <f>(C5/C72)</f>
         <v>1.3761467889908258E-2</v>
       </c>
-      <c r="E5" s="8"/>
+      <c r="E5" s="7"/>
       <c r="F5" s="6">
         <v>12</v>
       </c>
@@ -868,11 +867,11 @@
       <c r="C6" s="5">
         <v>40</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <f>(C6/C72)</f>
         <v>4.5871559633027525E-2</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="7"/>
       <c r="F6" s="6">
         <v>40</v>
       </c>
@@ -887,11 +886,11 @@
       <c r="C7" s="5">
         <v>9</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <f>(C7/C72)</f>
         <v>1.0321100917431193E-2</v>
       </c>
-      <c r="E7" s="8"/>
+      <c r="E7" s="7"/>
       <c r="F7" s="6">
         <v>9</v>
       </c>
@@ -906,11 +905,11 @@
       <c r="C8" s="5">
         <v>43</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <f>(C8/C72)</f>
         <v>4.931192660550459E-2</v>
       </c>
-      <c r="E8" s="8"/>
+      <c r="E8" s="7"/>
       <c r="F8" s="6">
         <v>43</v>
       </c>
@@ -925,11 +924,11 @@
       <c r="C9" s="5">
         <v>2</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <f>(C9/C72)</f>
         <v>2.2935779816513763E-3</v>
       </c>
-      <c r="E9" s="8"/>
+      <c r="E9" s="7"/>
       <c r="F9" s="6">
         <v>2</v>
       </c>
@@ -944,11 +943,11 @@
       <c r="C10" s="5">
         <v>3</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <f>(C10/C72)</f>
         <v>3.4403669724770644E-3</v>
       </c>
-      <c r="E10" s="8"/>
+      <c r="E10" s="7"/>
       <c r="F10" s="6">
         <v>3</v>
       </c>
@@ -963,11 +962,11 @@
       <c r="C11" s="5">
         <v>13</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <f>(C11/C72)</f>
         <v>1.4908256880733946E-2</v>
       </c>
-      <c r="E11" s="8"/>
+      <c r="E11" s="7"/>
       <c r="F11" s="6">
         <v>13</v>
       </c>
@@ -982,11 +981,11 @@
       <c r="C12" s="5">
         <v>1</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <f>(C12/C72)</f>
         <v>1.1467889908256881E-3</v>
       </c>
-      <c r="E12" s="8"/>
+      <c r="E12" s="7"/>
       <c r="F12" s="6">
         <v>1</v>
       </c>
@@ -1001,11 +1000,11 @@
       <c r="C13" s="5">
         <v>23</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <f>(C13/C72)</f>
         <v>2.6376146788990827E-2</v>
       </c>
-      <c r="E13" s="8"/>
+      <c r="E13" s="7"/>
       <c r="F13" s="6">
         <v>23</v>
       </c>
@@ -1020,11 +1019,11 @@
       <c r="C14" s="5">
         <v>40</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="9">
         <f>(C14/C72)</f>
         <v>4.5871559633027525E-2</v>
       </c>
-      <c r="E14" s="8"/>
+      <c r="E14" s="7"/>
       <c r="F14" s="6">
         <v>40</v>
       </c>
@@ -1039,11 +1038,11 @@
       <c r="C15" s="5">
         <v>10</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="9">
         <f>C15/C72</f>
         <v>1.1467889908256881E-2</v>
       </c>
-      <c r="E15" s="8"/>
+      <c r="E15" s="7"/>
       <c r="F15" s="6">
         <v>10</v>
       </c>
@@ -1058,11 +1057,11 @@
       <c r="C16" s="5">
         <v>17</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="9">
         <f>C16/C72</f>
         <v>1.9495412844036698E-2</v>
       </c>
-      <c r="E16" s="8"/>
+      <c r="E16" s="7"/>
       <c r="F16" s="6">
         <v>17</v>
       </c>
@@ -1077,11 +1076,11 @@
       <c r="C17" s="5">
         <v>16</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="9">
         <f>C17/C72</f>
         <v>1.834862385321101E-2</v>
       </c>
-      <c r="E17" s="8"/>
+      <c r="E17" s="7"/>
       <c r="F17" s="6">
         <v>16</v>
       </c>
@@ -1096,11 +1095,11 @@
       <c r="C18" s="5">
         <v>6</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="9">
         <f>C18/C72</f>
         <v>6.8807339449541288E-3</v>
       </c>
-      <c r="E18" s="8"/>
+      <c r="E18" s="7"/>
       <c r="F18" s="6">
         <v>6</v>
       </c>
@@ -1115,11 +1114,11 @@
       <c r="C19" s="5">
         <v>5</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="9">
         <f>C19/C72</f>
         <v>5.7339449541284407E-3</v>
       </c>
-      <c r="E19" s="8"/>
+      <c r="E19" s="7"/>
       <c r="F19" s="6">
         <v>5</v>
       </c>
@@ -1134,11 +1133,11 @@
       <c r="C20" s="5">
         <v>39</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="9">
         <f>C20/C72</f>
         <v>4.4724770642201837E-2</v>
       </c>
-      <c r="E20" s="8"/>
+      <c r="E20" s="7"/>
       <c r="F20" s="6">
         <v>39</v>
       </c>
@@ -1153,11 +1152,11 @@
       <c r="C21" s="5">
         <v>11</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="9">
         <f>C21/C72</f>
         <v>1.261467889908257E-2</v>
       </c>
-      <c r="E21" s="8"/>
+      <c r="E21" s="7"/>
       <c r="F21" s="6">
         <v>11</v>
       </c>
@@ -1172,11 +1171,11 @@
       <c r="C22" s="5">
         <v>11</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="9">
         <f>C22/C72</f>
         <v>1.261467889908257E-2</v>
       </c>
-      <c r="E22" s="8"/>
+      <c r="E22" s="7"/>
       <c r="F22" s="6">
         <v>11</v>
       </c>
@@ -1191,11 +1190,11 @@
       <c r="C23" s="5">
         <v>19</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="9">
         <f>C23/C72</f>
         <v>2.1788990825688075E-2</v>
       </c>
-      <c r="E23" s="8"/>
+      <c r="E23" s="7"/>
       <c r="F23" s="6">
         <v>19</v>
       </c>
@@ -1210,11 +1209,11 @@
       <c r="C24" s="5">
         <v>2</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="9">
         <f>C24/C72</f>
         <v>2.2935779816513763E-3</v>
       </c>
-      <c r="E24" s="8"/>
+      <c r="E24" s="7"/>
       <c r="F24" s="6">
         <v>2</v>
       </c>
@@ -1229,11 +1228,11 @@
       <c r="C25" s="5">
         <v>36</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="9">
         <f>C25/C72</f>
         <v>4.1284403669724773E-2</v>
       </c>
-      <c r="E25" s="8"/>
+      <c r="E25" s="7"/>
       <c r="F25" s="6">
         <v>36</v>
       </c>
@@ -1248,11 +1247,11 @@
       <c r="C26" s="5">
         <v>16</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="9">
         <f>C26/C72</f>
         <v>1.834862385321101E-2</v>
       </c>
-      <c r="E26" s="8"/>
+      <c r="E26" s="7"/>
       <c r="F26" s="6">
         <v>16</v>
       </c>
@@ -1267,11 +1266,11 @@
       <c r="C27" s="5">
         <v>14</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D27" s="9">
         <f>C27/C72</f>
         <v>1.6055045871559634E-2</v>
       </c>
-      <c r="E27" s="8"/>
+      <c r="E27" s="7"/>
       <c r="F27" s="6">
         <v>14</v>
       </c>
@@ -1286,11 +1285,11 @@
       <c r="C28" s="5">
         <v>16</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="9">
         <f>C28/C72</f>
         <v>1.834862385321101E-2</v>
       </c>
-      <c r="E28" s="8"/>
+      <c r="E28" s="7"/>
       <c r="F28" s="6">
         <v>16</v>
       </c>
@@ -1305,11 +1304,11 @@
       <c r="C29" s="5">
         <v>1</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29" s="9">
         <f>C29/C72</f>
         <v>1.1467889908256881E-3</v>
       </c>
-      <c r="E29" s="8"/>
+      <c r="E29" s="7"/>
       <c r="F29" s="6">
         <v>1</v>
       </c>
@@ -1324,11 +1323,11 @@
       <c r="C30" s="5">
         <v>27</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D30" s="9">
         <f>C30/C72</f>
         <v>3.096330275229358E-2</v>
       </c>
-      <c r="E30" s="8"/>
+      <c r="E30" s="7"/>
       <c r="F30" s="6">
         <v>27</v>
       </c>
@@ -1343,11 +1342,11 @@
       <c r="C31" s="5">
         <v>2</v>
       </c>
-      <c r="D31" s="10">
+      <c r="D31" s="9">
         <f>C31/C72</f>
         <v>2.2935779816513763E-3</v>
       </c>
-      <c r="E31" s="8"/>
+      <c r="E31" s="7"/>
       <c r="F31" s="6">
         <v>2</v>
       </c>
@@ -1362,11 +1361,11 @@
       <c r="C32" s="5">
         <v>9</v>
       </c>
-      <c r="D32" s="10">
+      <c r="D32" s="9">
         <f>C32/C72</f>
         <v>1.0321100917431193E-2</v>
       </c>
-      <c r="E32" s="8"/>
+      <c r="E32" s="7"/>
       <c r="F32" s="6">
         <v>9</v>
       </c>
@@ -1381,11 +1380,11 @@
       <c r="C33" s="5">
         <v>14</v>
       </c>
-      <c r="D33" s="10">
+      <c r="D33" s="9">
         <f>C33/C72</f>
         <v>1.6055045871559634E-2</v>
       </c>
-      <c r="E33" s="8"/>
+      <c r="E33" s="7"/>
       <c r="F33" s="6">
         <v>14</v>
       </c>
@@ -1400,11 +1399,11 @@
       <c r="C34" s="5">
         <v>22</v>
       </c>
-      <c r="D34" s="10">
+      <c r="D34" s="9">
         <f>C34/C72</f>
         <v>2.5229357798165139E-2</v>
       </c>
-      <c r="E34" s="8"/>
+      <c r="E34" s="7"/>
       <c r="F34" s="6">
         <v>22</v>
       </c>
@@ -1419,11 +1418,11 @@
       <c r="C35" s="5">
         <v>12</v>
       </c>
-      <c r="D35" s="10">
+      <c r="D35" s="9">
         <f>C35/C72</f>
         <v>1.3761467889908258E-2</v>
       </c>
-      <c r="E35" s="8"/>
+      <c r="E35" s="7"/>
       <c r="F35" s="6">
         <v>12</v>
       </c>
@@ -1438,11 +1437,11 @@
       <c r="C36" s="5">
         <v>1</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D36" s="9">
         <f>C36/C72</f>
         <v>1.1467889908256881E-3</v>
       </c>
-      <c r="E36" s="8"/>
+      <c r="E36" s="7"/>
       <c r="F36" s="6">
         <v>1</v>
       </c>
@@ -1457,13 +1456,13 @@
       <c r="C37" s="5">
         <v>8</v>
       </c>
-      <c r="D37" s="10">
+      <c r="D37" s="9">
         <f>C37/C72</f>
         <v>9.1743119266055051E-3</v>
       </c>
-      <c r="E37" s="8"/>
+      <c r="E37" s="7"/>
       <c r="F37" s="6">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1476,13 +1475,13 @@
       <c r="C38" s="5">
         <v>2</v>
       </c>
-      <c r="D38" s="10">
+      <c r="D38" s="9">
         <f>C38/C72</f>
         <v>2.2935779816513763E-3</v>
       </c>
-      <c r="E38" s="8"/>
+      <c r="E38" s="7"/>
       <c r="F38" s="6">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1495,11 +1494,11 @@
       <c r="C39" s="5">
         <v>9</v>
       </c>
-      <c r="D39" s="10">
+      <c r="D39" s="9">
         <f>C39/C72</f>
         <v>1.0321100917431193E-2</v>
       </c>
-      <c r="E39" s="8"/>
+      <c r="E39" s="7"/>
       <c r="F39" s="6">
         <v>9</v>
       </c>
@@ -1514,11 +1513,11 @@
       <c r="C40" s="5">
         <v>18</v>
       </c>
-      <c r="D40" s="10">
+      <c r="D40" s="9">
         <f>C40/C72</f>
         <v>2.0642201834862386E-2</v>
       </c>
-      <c r="E40" s="8"/>
+      <c r="E40" s="7"/>
       <c r="F40" s="6">
         <v>18</v>
       </c>
@@ -1533,11 +1532,11 @@
       <c r="C41" s="5">
         <v>14</v>
       </c>
-      <c r="D41" s="10">
+      <c r="D41" s="9">
         <f>C41/C72</f>
         <v>1.6055045871559634E-2</v>
       </c>
-      <c r="E41" s="8"/>
+      <c r="E41" s="7"/>
       <c r="F41" s="6">
         <v>14</v>
       </c>
@@ -1552,12 +1551,14 @@
       <c r="C42" s="5">
         <v>27</v>
       </c>
-      <c r="D42" s="10">
+      <c r="D42" s="9">
         <f>C42/C72</f>
         <v>3.096330275229358E-2</v>
       </c>
-      <c r="E42" s="8"/>
-      <c r="F42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="6">
+        <v>27</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
@@ -1569,12 +1570,14 @@
       <c r="C43" s="5">
         <v>45</v>
       </c>
-      <c r="D43" s="10">
+      <c r="D43" s="9">
         <f>C43/C72</f>
         <v>5.1605504587155966E-2</v>
       </c>
-      <c r="E43" s="8"/>
-      <c r="F43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="6">
+        <v>45</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
@@ -1586,12 +1589,14 @@
       <c r="C44" s="5">
         <v>7</v>
       </c>
-      <c r="D44" s="10">
+      <c r="D44" s="9">
         <f>C44/C72</f>
         <v>8.027522935779817E-3</v>
       </c>
-      <c r="E44" s="8"/>
-      <c r="F44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="6">
+        <v>7</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
@@ -1603,12 +1608,14 @@
       <c r="C45" s="5">
         <v>1</v>
       </c>
-      <c r="D45" s="10">
+      <c r="D45" s="9">
         <f>C45/C72</f>
         <v>1.1467889908256881E-3</v>
       </c>
-      <c r="E45" s="8"/>
-      <c r="F45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
@@ -1620,12 +1627,14 @@
       <c r="C46" s="5">
         <v>15</v>
       </c>
-      <c r="D46" s="10">
+      <c r="D46" s="9">
         <f>C46/C72</f>
         <v>1.7201834862385322E-2</v>
       </c>
-      <c r="E46" s="8"/>
-      <c r="F46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="6">
+        <v>15</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
@@ -1637,12 +1646,14 @@
       <c r="C47" s="5">
         <v>12</v>
       </c>
-      <c r="D47" s="10">
+      <c r="D47" s="9">
         <f>C47/C72</f>
         <v>1.3761467889908258E-2</v>
       </c>
-      <c r="E47" s="8"/>
-      <c r="F47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="6">
+        <v>12</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
@@ -1654,12 +1665,14 @@
       <c r="C48" s="5">
         <v>1</v>
       </c>
-      <c r="D48" s="10">
+      <c r="D48" s="9">
         <f>C48/C72</f>
         <v>1.1467889908256881E-3</v>
       </c>
-      <c r="E48" s="8"/>
-      <c r="F48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
@@ -1671,12 +1684,14 @@
       <c r="C49" s="5">
         <v>24</v>
       </c>
-      <c r="D49" s="10">
+      <c r="D49" s="9">
         <f>C49/C72</f>
         <v>2.7522935779816515E-2</v>
       </c>
-      <c r="E49" s="8"/>
-      <c r="F49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="6">
+        <v>24</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
@@ -1688,12 +1703,14 @@
       <c r="C50" s="5">
         <v>2</v>
       </c>
-      <c r="D50" s="10">
+      <c r="D50" s="9">
         <f>C50/C72</f>
         <v>2.2935779816513763E-3</v>
       </c>
-      <c r="E50" s="8"/>
-      <c r="F50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
@@ -1705,12 +1722,14 @@
       <c r="C51" s="5">
         <v>6</v>
       </c>
-      <c r="D51" s="10">
+      <c r="D51" s="9">
         <f>C51/C72</f>
         <v>6.8807339449541288E-3</v>
       </c>
-      <c r="E51" s="8"/>
-      <c r="F51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="6">
+        <v>6</v>
+      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
@@ -1722,12 +1741,14 @@
       <c r="C52" s="5">
         <v>2</v>
       </c>
-      <c r="D52" s="10">
+      <c r="D52" s="9">
         <f>C52/C72</f>
         <v>2.2935779816513763E-3</v>
       </c>
-      <c r="E52" s="8"/>
-      <c r="F52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
@@ -1739,12 +1760,14 @@
       <c r="C53" s="5">
         <v>22</v>
       </c>
-      <c r="D53" s="10">
+      <c r="D53" s="9">
         <f>C53/C72</f>
         <v>2.5229357798165139E-2</v>
       </c>
-      <c r="E53" s="8"/>
-      <c r="F53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="6">
+        <v>22</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
@@ -1756,12 +1779,14 @@
       <c r="C54" s="5">
         <v>8</v>
       </c>
-      <c r="D54" s="10">
+      <c r="D54" s="9">
         <f>C54/C72</f>
         <v>9.1743119266055051E-3</v>
       </c>
-      <c r="E54" s="8"/>
-      <c r="F54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="6">
+        <v>8</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
@@ -1773,12 +1798,14 @@
       <c r="C55" s="5">
         <v>1</v>
       </c>
-      <c r="D55" s="10">
+      <c r="D55" s="9">
         <f>C55/C72</f>
         <v>1.1467889908256881E-3</v>
       </c>
-      <c r="E55" s="8"/>
-      <c r="F55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
@@ -1790,12 +1817,14 @@
       <c r="C56" s="5">
         <v>3</v>
       </c>
-      <c r="D56" s="10">
+      <c r="D56" s="9">
         <f>C56/C72</f>
         <v>3.4403669724770644E-3</v>
       </c>
-      <c r="E56" s="8"/>
-      <c r="F56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
@@ -1807,12 +1836,14 @@
       <c r="C57" s="5">
         <v>7</v>
       </c>
-      <c r="D57" s="10">
+      <c r="D57" s="9">
         <f>C57/C72</f>
         <v>8.027522935779817E-3</v>
       </c>
-      <c r="E57" s="8"/>
-      <c r="F57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="6">
+        <v>7</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
@@ -1824,12 +1855,14 @@
       <c r="C58" s="5">
         <v>3</v>
       </c>
-      <c r="D58" s="10">
+      <c r="D58" s="9">
         <f>C58/C72</f>
         <v>3.4403669724770644E-3</v>
       </c>
-      <c r="E58" s="8"/>
-      <c r="F58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="5">
@@ -1841,12 +1874,14 @@
       <c r="C59" s="5">
         <v>4</v>
       </c>
-      <c r="D59" s="10">
+      <c r="D59" s="9">
         <f>C59/C72</f>
         <v>4.5871559633027525E-3</v>
       </c>
-      <c r="E59" s="8"/>
-      <c r="F59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="6">
+        <v>4</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
@@ -1858,12 +1893,14 @@
       <c r="C60" s="5">
         <v>6</v>
       </c>
-      <c r="D60" s="10">
+      <c r="D60" s="9">
         <f>C60/C72</f>
         <v>6.8807339449541288E-3</v>
       </c>
-      <c r="E60" s="8"/>
-      <c r="F60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="6">
+        <v>6</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="5">
@@ -1875,12 +1912,14 @@
       <c r="C61" s="5">
         <v>2</v>
       </c>
-      <c r="D61" s="10">
+      <c r="D61" s="9">
         <f>C61/C72</f>
         <v>2.2935779816513763E-3</v>
       </c>
-      <c r="E61" s="8"/>
-      <c r="F61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="5">
@@ -1892,12 +1931,14 @@
       <c r="C62" s="5">
         <v>2</v>
       </c>
-      <c r="D62" s="10">
+      <c r="D62" s="9">
         <f>C62/C72</f>
         <v>2.2935779816513763E-3</v>
       </c>
-      <c r="E62" s="8"/>
-      <c r="F62" s="7"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="5">
@@ -1909,12 +1950,14 @@
       <c r="C63" s="5">
         <v>1</v>
       </c>
-      <c r="D63" s="10">
+      <c r="D63" s="9">
         <f>C63/C72</f>
         <v>1.1467889908256881E-3</v>
       </c>
-      <c r="E63" s="8"/>
-      <c r="F63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="5">
@@ -1926,12 +1969,14 @@
       <c r="C64" s="5">
         <v>11</v>
       </c>
-      <c r="D64" s="10">
+      <c r="D64" s="9">
         <f>C64/C72</f>
         <v>1.261467889908257E-2</v>
       </c>
-      <c r="E64" s="8"/>
-      <c r="F64" s="7"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="6">
+        <v>11</v>
+      </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="5">
@@ -1943,12 +1988,14 @@
       <c r="C65" s="5">
         <v>4</v>
       </c>
-      <c r="D65" s="10">
+      <c r="D65" s="9">
         <f>C65/C72</f>
         <v>4.5871559633027525E-3</v>
       </c>
-      <c r="E65" s="8"/>
-      <c r="F65" s="7"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="6">
+        <v>4</v>
+      </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="5">
@@ -1960,11 +2007,11 @@
       <c r="C66" s="5">
         <v>6</v>
       </c>
-      <c r="D66" s="10">
+      <c r="D66" s="9">
         <f>C66/C72</f>
         <v>6.8807339449541288E-3</v>
       </c>
-      <c r="E66" s="8"/>
+      <c r="E66" s="7"/>
       <c r="F66" s="6">
         <v>6</v>
       </c>
@@ -1979,12 +2026,14 @@
       <c r="C67" s="5">
         <v>38</v>
       </c>
-      <c r="D67" s="10">
+      <c r="D67" s="9">
         <f>C67/C72</f>
         <v>4.3577981651376149E-2</v>
       </c>
-      <c r="E67" s="8"/>
-      <c r="F67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="6">
+        <v>38</v>
+      </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="5">
@@ -1996,12 +2045,14 @@
       <c r="C68" s="5">
         <v>4</v>
       </c>
-      <c r="D68" s="10">
+      <c r="D68" s="9">
         <f>C68/C72</f>
         <v>4.5871559633027525E-3</v>
       </c>
-      <c r="E68" s="8"/>
-      <c r="F68" s="7"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="6">
+        <v>4</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="5">
@@ -2013,12 +2064,14 @@
       <c r="C69" s="5">
         <v>25</v>
       </c>
-      <c r="D69" s="10">
+      <c r="D69" s="9">
         <f>C69/C72</f>
         <v>2.8669724770642203E-2</v>
       </c>
-      <c r="E69" s="8"/>
-      <c r="F69" s="7"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="6">
+        <v>25</v>
+      </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="5">
@@ -2030,12 +2083,14 @@
       <c r="C70" s="5">
         <v>19</v>
       </c>
-      <c r="D70" s="10">
+      <c r="D70" s="9">
         <f>C70/C72</f>
         <v>2.1788990825688075E-2</v>
       </c>
-      <c r="E70" s="8"/>
-      <c r="F70" s="7"/>
+      <c r="E70" s="7"/>
+      <c r="F70" s="6">
+        <v>19</v>
+      </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
@@ -2045,16 +2100,16 @@
         <f>SUM(C2:C70)</f>
         <v>872</v>
       </c>
-      <c r="D72" s="10">
+      <c r="D72" s="9">
         <f>C72/C72</f>
         <v>1</v>
       </c>
-      <c r="E72" s="12">
+      <c r="E72" s="11">
         <v>1</v>
       </c>
-      <c r="F72" s="10">
+      <c r="F72" s="9">
         <f>(SUM(F2:F70)/SUM(C2:C70))</f>
-        <v>0.65252293577981646</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>